<commit_message>
Adding LightGBM and Catboost
</commit_message>
<xml_diff>
--- a/Jupyter/Python/resultados_regressao.xlsx
+++ b/Jupyter/Python/resultados_regressao.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,38 +502,38 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-1.191778943135376</v>
+        <v>-1.191779160026281</v>
       </c>
       <c r="D2" t="n">
-        <v>9747.494045567568</v>
+        <v>9747.457259750538</v>
       </c>
       <c r="E2" t="n">
-        <v>17866.11471871991</v>
+        <v>17866.11560270452</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.4551661395074511</v>
+        <v>-0.4551661381186431</v>
       </c>
       <c r="G2" t="n">
-        <v>20544.3973470141</v>
+        <v>20544.39727538676</v>
       </c>
       <c r="H2" t="n">
-        <v>10278.90186859302</v>
+        <v>10278.90184040628</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[-5.36936069e+08 -4.84330910e+07 -6.09596730e+07 -3.33792394e+08
+          <t>[-5.36936080e+08 -4.84330921e+07 -6.09596707e+07 -3.33792368e+08
  -1.13024009e+09]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[-1.86960878 -0.19760903 -0.61686124  0.56700028 -0.15875192]</t>
+          <t>[-1.86960885 -0.19760905 -0.61686118  0.56700031 -0.15875193]</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[ -9896.10244932  -6241.48337997  -5617.34017232 -11961.72526973
- -17677.85807162]</t>
+          <t>[ -9896.10240574  -6241.48377845  -5617.34012575 -11961.72481999
+ -17677.85807211]</t>
         </is>
       </c>
     </row>
@@ -549,38 +549,38 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.7811137929032153</v>
+        <v>-0.7811135038951063</v>
       </c>
       <c r="D3" t="n">
-        <v>8855.467650887973</v>
+        <v>8855.464493685831</v>
       </c>
       <c r="E3" t="n">
-        <v>16105.62476659563</v>
+        <v>16105.62345992551</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.07832849704789982</v>
+        <v>-0.07832636867183637</v>
       </c>
       <c r="G3" t="n">
-        <v>17290.32578890672</v>
+        <v>17290.32346778754</v>
       </c>
       <c r="H3" t="n">
-        <v>8779.121488817058</v>
+        <v>8779.115747629901</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>[-3.76445292e+08 -3.31225718e+07 -5.31551443e+07 -3.41162024e+08
+          <t>[-3.76445292e+08 -3.31225718e+07 -5.31547431e+07 -3.41162024e+08
  -6.90891797e+08]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[-1.01187959  0.18097544 -0.40985816  0.5574403   0.29167952]</t>
+          <t>[-1.01187959  0.18097544 -0.40984752  0.5574403   0.29167952]</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>[ -8565.76416667  -4887.84967665  -5681.05342046 -11750.18556452
- -13010.7546158 ]</t>
+          <t>[ -8565.76416386  -4887.84968104  -5681.0247185  -11750.18556298
+ -13010.75461177]</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
         <v>17855.20772481208</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.3835476171442401</v>
+        <v>-0.38354761714424</v>
       </c>
       <c r="G4" t="n">
         <v>19943.25743860208</v>
@@ -690,38 +690,38 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1939396840870856</v>
+        <v>0.160688677823154</v>
       </c>
       <c r="D6" t="n">
-        <v>5326.905</v>
+        <v>5589.49880952381</v>
       </c>
       <c r="E6" t="n">
-        <v>10834.66563782427</v>
+        <v>11055.87917927197</v>
       </c>
       <c r="F6" t="n">
-        <v>0.03412170666511516</v>
+        <v>-0.01202178513521324</v>
       </c>
       <c r="G6" t="n">
-        <v>17891.92617630059</v>
+        <v>18678.59998461572</v>
       </c>
       <c r="H6" t="n">
-        <v>8003.849047368421</v>
+        <v>8265.572647368421</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>[-5.06138936e+08 -6.17561279e+06 -2.78336720e+07 -5.37589130e+08
- -5.22867760e+08]</t>
+          <t>[-5.06789192e+08 -1.19083116e+07 -2.57607087e+07 -5.28089041e+08
+ -6.71903234e+08]</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>[-1.70501615  0.84729511  0.26175481  0.30263257  0.46394219]</t>
+          <t>[-1.70849139  0.7055422   0.31673696  0.3149562   0.3111471 ]</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>[ -9740.039       -1773.568       -3473.0635     -13288.75894737
- -11743.81578947]</t>
+          <t>[ -9917.2135      -2332.8615      -3178.4635     -12616.44315789
+ -13282.88157895]</t>
         </is>
       </c>
     </row>
@@ -737,38 +737,38 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.135952738150742</v>
+        <v>0.2667827799071745</v>
       </c>
       <c r="D7" t="n">
-        <v>6019.953280952376</v>
+        <v>5683.118419047614</v>
       </c>
       <c r="E7" t="n">
-        <v>11217.61401277423</v>
+        <v>10333.51492798416</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3461450699913592</v>
+        <v>0.37054827230222</v>
       </c>
       <c r="G7" t="n">
-        <v>15120.50871324514</v>
+        <v>15032.85774066459</v>
       </c>
       <c r="H7" t="n">
-        <v>6550.177976842104</v>
+        <v>6483.545771421052</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>[-3.03644636e+08 -8.03532677e+06 -2.03188805e+07 -2.83993559e+08
- -5.27156517e+08]</t>
+          <t>[-2.88786445e+08 -8.02524460e+06 -1.85820434e+07 -2.84849348e+08
+ -5.29690978e+08]</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>[-0.62280272  0.80130981  0.46107306  0.63159996  0.45954524]</t>
+          <t>[-0.5433944   0.80155912  0.50713998  0.63048982  0.45694685]</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>[ -7083.292045    -2024.7389      -2838.875355    -9021.54457895
- -11782.43900526]</t>
+          <t>[ -7037.863755    -2096.66447     -2724.67799     -9098.60597895
+ -11459.91666316]</t>
         </is>
       </c>
     </row>
@@ -784,38 +784,38 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.4049979082762655</v>
+        <v>0.4328762177266555</v>
       </c>
       <c r="D8" t="n">
-        <v>4704.874545321021</v>
+        <v>4559.395693542933</v>
       </c>
       <c r="E8" t="n">
-        <v>9308.74190943549</v>
+        <v>9088.049273469329</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1941739742514308</v>
+        <v>0.1824812057294804</v>
       </c>
       <c r="G8" t="n">
-        <v>16183.67470087206</v>
+        <v>16160.67192591208</v>
       </c>
       <c r="H8" t="n">
-        <v>6878.785482811317</v>
+        <v>6996.381219108363</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>[-4.01095363e+08 -7.93438434e+06 -2.71950342e+07 -2.67098117e+08
- -6.06233735e+08]</t>
+          <t>[-4.08541864e+08 -7.83030482e+06 -2.84367527e+07 -2.70481201e+08
+ -5.90546463e+08]</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>[-1.14361978  0.80380583  0.27869369  0.65351694  0.3784732 ]</t>
+          <t>[-1.18341696  0.80637941  0.24575903  0.64912836  0.3945562 ]</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>[ -7814.82794089  -2074.26619594  -3126.81742206  -8492.64880766
- -12885.36704751]</t>
+          <t>[ -7910.78035296  -2054.01274835  -3212.11590815  -8928.71489846
+ -12876.28218763]</t>
         </is>
       </c>
     </row>
@@ -874,133 +874,227 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>LightGBM</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>-0.5062336308909425</v>
+      </c>
+      <c r="D10" t="n">
+        <v>9402.940989458264</v>
+      </c>
+      <c r="E10" t="n">
+        <v>14810.77939627252</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-0.7411596952515552</v>
+      </c>
+      <c r="G10" t="n">
+        <v>19530.44383360109</v>
+      </c>
+      <c r="H10" t="n">
+        <v>10822.51912859489</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>[-2.76605469e+08 -5.80258760e+07 -1.58249892e+08 -5.34481653e+08
+ -8.79828292e+08]</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>[-0.47829421 -0.43481061 -3.19733412  0.30666363  0.09797685]</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>[-10018.5647826   -5643.43607803  -9006.64071117 -11911.40488544
+ -17532.54918574]</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>CatBoost</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.4032481595475715</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4812.576743866931</v>
+      </c>
+      <c r="E11" t="n">
+        <v>9322.419174141065</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.3522514500934445</v>
+      </c>
+      <c r="G11" t="n">
+        <v>14858.62242451191</v>
+      </c>
+      <c r="H11" t="n">
+        <v>6530.750213051405</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>[-2.70000843e+08 -1.13316167e+07 -2.45974495e+07 -1.65618951e+08
+ -6.32344441e+08]</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>[-0.44299636  0.71980218  0.34759062  0.785157    0.35170381]</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>[ -5841.93850766  -2563.5335398   -3167.97967961  -8365.2116056
+ -12715.08773258]</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>SVR (Linear Kernel)</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C12" t="n">
         <v>-0.08737487153970336</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D12" t="n">
         <v>7003.501188517066</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E12" t="n">
         <v>12584.07764949718</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F12" t="n">
         <v>-0.1062014174225997</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G12" t="n">
         <v>21918.16352119195</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H12" t="n">
         <v>9820.227627208802</v>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>[-2.04477250e+08 -4.02385224e+07 -3.89206864e+07 -8.78982548e+08
  -1.23941045e+09]</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>[-0.09281113  0.00501875 -0.03231113 -0.1402273  -0.27067626]</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>[ -7657.71394167  -4773.9660222   -4228.52997215 -13363.10566351
  -19077.82253651]</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Dataset 1</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>SVR (RBF Kernel)</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C13" t="n">
         <v>-0.08737487153970336</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D13" t="n">
         <v>7003.501188517066</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E13" t="n">
         <v>12584.07764949718</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F13" t="n">
         <v>-0.1062014174225997</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G13" t="n">
         <v>21918.16352119195</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H13" t="n">
         <v>9820.227627208802</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>[-2.04477250e+08 -4.02385224e+07 -3.89206864e+07 -8.78982548e+08
  -1.23941045e+09]</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>[-0.09281113  0.00501875 -0.03231113 -0.1402273  -0.27067626]</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>[ -7657.71394167  -4773.9660222   -4228.52997215 -13363.10566351
  -19077.82253651]</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Dataset 1</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>SVR (Sigmoid Kernel)</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C14" t="n">
         <v>-0.08036218691983588</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D14" t="n">
         <v>6964.719479724569</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E14" t="n">
         <v>12543.43347378073</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F14" t="n">
         <v>-0.1006732588117087</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G14" t="n">
         <v>21889.68805299561</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H14" t="n">
         <v>9794.523531732368</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>[-2.04145448e+08 -3.97724889e+07 -3.86078033e+07 -8.76080697e+08
  -1.23718578e+09]</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>[-0.09103784  0.01654239 -0.02401239 -0.13646298 -0.26839547]</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>[ -7642.83911925  -4746.31506427  -4212.31752338 -13319.68168976
  -19051.464262  ]</t>

</xml_diff>

<commit_message>
Adding function to store different encoders
</commit_message>
<xml_diff>
--- a/Jupyter/Python/resultados_regressao.xlsx
+++ b/Jupyter/Python/resultados_regressao.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,50 +441,55 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Encoder</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>R2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>MAE</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>RMSE</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>CV R2</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>CV RMSE</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>CV MAE</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>CV RMSE por fold</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>CV R2 por fold</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>CV MAE por fold</t>
         </is>
@@ -498,39 +503,44 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>onehot</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Regressao Linear</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>-1.191779160026281</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>9747.457259750538</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>17866.11560270452</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>-0.4551661381186431</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>20544.39727538676</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>10278.90184040628</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>[-5.36936080e+08 -4.84330921e+07 -6.09596707e+07 -3.33792368e+08
  -1.13024009e+09]</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>[-1.86960885 -0.19760905 -0.61686118  0.56700031 -0.15875193]</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>[ -9896.10240574  -6241.48377845  -5617.34012575 -11961.72481999
  -17677.85807211]</t>
@@ -545,39 +555,44 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>onehot</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Ridge</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>-0.7811135038951063</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>8855.464493685831</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>16105.62345992551</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>-0.07832636867183637</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>17290.32346778754</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>8779.115747629901</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>[-3.76445292e+08 -3.31225718e+07 -5.31547431e+07 -3.41162024e+08
  -6.90891797e+08]</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>[-1.01187959  0.18097544 -0.40984752  0.5574403   0.29167952]</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>[ -8565.76416386  -4887.84968104  -5681.0247185  -11750.18556298
  -13010.75461177]</t>
@@ -592,39 +607,44 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>onehot</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Lasso</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>-1.189103663936121</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>9732.808719593968</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>17855.20772481208</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>-0.38354761714424</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>19943.25743860208</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>9807.728526960354</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>[-4.94040160e+08 -4.77261766e+07 -6.05320644e+07 -2.58806791e+08
  -1.12756239e+09]</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>[-1.64035528 -0.1801291  -0.60551958  0.66427255 -0.15600669]</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>[ -8529.24449514  -6181.36508366  -5601.86556906 -11103.01550649
  -17623.15198045]</t>
@@ -639,39 +659,44 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>onehot</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>ElasticNet</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>0.342469142165772</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>7397.197215428671</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>9785.653024225001</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>-0.001095598073094162</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>18691.39407988569</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>10303.0258197788</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>[-1.43475822e+08 -3.80155820e+07 -6.04523021e+07 -5.60340303e+08
  -9.44557054e+08]</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>[ 0.23320577  0.05998558 -0.60340401  0.27311946  0.03161521]</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>[ -8349.24679487  -5397.95820809  -7216.00015016 -12770.67073553
  -17781.25321025]</t>
@@ -686,42 +711,47 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>onehot</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>Arvore de Decisao</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>0.160688677823154</v>
-      </c>
       <c r="D6" t="n">
-        <v>5589.49880952381</v>
+        <v>0.1902533389644809</v>
       </c>
       <c r="E6" t="n">
-        <v>11055.87917927197</v>
+        <v>5341.505476190476</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.01202178513521324</v>
+        <v>10859.41239407207</v>
       </c>
       <c r="G6" t="n">
-        <v>18678.59998461572</v>
+        <v>0.3410851386779976</v>
       </c>
       <c r="H6" t="n">
-        <v>8265.572647368421</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>[-5.06789192e+08 -1.19083116e+07 -2.57607087e+07 -5.28089041e+08
- -6.71903234e+08]</t>
-        </is>
+        <v>16353.68763897397</v>
+      </c>
+      <c r="I6" t="n">
+        <v>7251.092378947369</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>[-1.70849139  0.7055422   0.31673696  0.3149562   0.3111471 ]</t>
+          <t>[-1.46487313e+08 -2.11219306e+07 -2.59618498e+07 -4.71749195e+08
+ -6.71895209e+08]</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>[ -9917.2135      -2332.8615      -3178.4635     -12616.44315789
- -13282.88157895]</t>
+          <t>[0.21711111 0.47771628 0.31140201 0.38804097 0.31115532]</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>[ -5674.2225      -3103.968       -3192.9135     -11036.85526316
+ -13247.50263158]</t>
         </is>
       </c>
     </row>
@@ -733,42 +763,47 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>onehot</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>Random Forest</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>0.2667827799071745</v>
-      </c>
       <c r="D7" t="n">
-        <v>5683.118419047614</v>
+        <v>-0.2128334802360237</v>
       </c>
       <c r="E7" t="n">
-        <v>10333.51492798416</v>
+        <v>6786.339497619042</v>
       </c>
       <c r="F7" t="n">
-        <v>0.37054827230222</v>
+        <v>13290.22494555015</v>
       </c>
       <c r="G7" t="n">
-        <v>15032.85774066459</v>
+        <v>0.344922087615741</v>
       </c>
       <c r="H7" t="n">
-        <v>6483.545771421052</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>[-2.88786445e+08 -8.02524460e+06 -1.85820434e+07 -2.84849348e+08
- -5.29690978e+08]</t>
-        </is>
+        <v>14918.77776147562</v>
+      </c>
+      <c r="I7" t="n">
+        <v>6402.480938157893</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>[-0.5433944   0.80155912  0.50713998  0.63048982  0.45694685]</t>
+          <t>[-3.14597134e+08 -8.58957120e+06 -1.92263023e+07 -3.00887103e+08
+ -4.69549539e+08]</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>[ -7037.863755    -2096.66447     -2724.67799     -9098.60597895
- -11459.91666316]</t>
+          <t>[-0.68133741  0.78760497  0.49005201  0.60968544  0.51860544]</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>[ -7387.206105    -2065.758205    -2802.203865    -8930.18904737
+ -10827.04746842]</t>
         </is>
       </c>
     </row>
@@ -780,42 +815,47 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>onehot</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>Gradient Boosting</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>0.4328762177266555</v>
-      </c>
       <c r="D8" t="n">
-        <v>4559.395693542933</v>
+        <v>0.415519116077802</v>
       </c>
       <c r="E8" t="n">
-        <v>9088.049273469329</v>
+        <v>4631.970034285237</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1824812057294804</v>
+        <v>9226.073263353755</v>
       </c>
       <c r="G8" t="n">
-        <v>16160.67192591208</v>
+        <v>0.2470576331221443</v>
       </c>
       <c r="H8" t="n">
-        <v>6996.381219108363</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>[-4.08541864e+08 -7.83030482e+06 -2.84367527e+07 -2.70481201e+08
- -5.90546463e+08]</t>
-        </is>
+        <v>16070.29642638487</v>
+      </c>
+      <c r="I8" t="n">
+        <v>6924.740470993594</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>[-1.18341696  0.80637941  0.24575903  0.64912836  0.3945562 ]</t>
+          <t>[-3.42753814e+08 -6.49125207e+06 -2.81805786e+07 -3.23684957e+08
+ -5.90161535e+08]</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>[ -7910.78035296  -2054.01274835  -3212.11590815  -8928.71489846
- -12876.28218763]</t>
+          <t>[-0.83181837  0.83949028  0.25255365  0.58011177  0.39495084]</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>[ -7224.71615991  -1968.30782832  -3138.92935799  -9450.7585784
+ -12840.99043035]</t>
         </is>
       </c>
     </row>
@@ -827,39 +867,44 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>onehot</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>XGBoost</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>0.6258352068970525</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>3682.10621673584</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>7381.815788899872</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>0.4363103065024265</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>14264.41864593009</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>6212.615042119718</v>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>[-1.83873811e+08 -8.04407659e+06 -2.79335274e+07 -2.87937945e+08
  -5.09578837e+08]</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>[0.01730218 0.80109346 0.2591063  0.62648325 0.47756635]</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>[ -5267.67803333  -1951.45250012  -3407.60198984  -9521.21791838
  -10915.12476893]</t>
@@ -874,39 +919,44 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>onehot</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>LightGBM</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>-0.5062336308909425</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>9402.940989458264</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>14810.77939627252</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>-0.7411596952515552</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>19530.44383360109</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>10822.51912859489</v>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>[-2.76605469e+08 -5.80258760e+07 -1.58249892e+08 -5.34481653e+08
  -8.79828292e+08]</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>[-0.47829421 -0.43481061 -3.19733412  0.30666363  0.09797685]</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>[-10018.5647826   -5643.43607803  -9006.64071117 -11911.40488544
  -17532.54918574]</t>
@@ -921,39 +971,44 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>onehot</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>CatBoost</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>0.4032481595475715</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>4812.576743866931</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>9322.419174141065</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>0.3522514500934445</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>14858.62242451191</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>6530.750213051405</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>[-2.70000843e+08 -1.13316167e+07 -2.45974495e+07 -1.65618951e+08
  -6.32344441e+08]</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>[-0.44299636  0.71980218  0.34759062  0.785157    0.35170381]</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>[ -5841.93850766  -2563.5335398   -3167.97967961  -8365.2116056
  -12715.08773258]</t>
@@ -968,92 +1023,102 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>onehot</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>SVR (Linear Kernel)</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
+        <v>-0.03328874256371361</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6629.315706845121</v>
+      </c>
+      <c r="F12" t="n">
+        <v>12267.11939030785</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-0.06225202916850434</v>
+      </c>
+      <c r="H12" t="n">
+        <v>21703.08592950889</v>
+      </c>
+      <c r="I12" t="n">
+        <v>9565.182123314622</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>[-2.03477029e+08 -3.58466103e+07 -3.67546654e+07 -8.49541734e+08
+ -1.22949965e+09]</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>[-0.08746554  0.11361792  0.02513923 -0.1020363  -0.26051545]</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>[ -7477.32311968  -4481.13756644  -4034.60548982 -12960.55953361
+ -18872.28490702]</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>onehot</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SVR (RBF Kernel)</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>-0.08737487153970336</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E13" t="n">
         <v>7003.501188517066</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F13" t="n">
         <v>12584.07764949718</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G13" t="n">
         <v>-0.1062014174225997</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H13" t="n">
         <v>21918.16352119195</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I13" t="n">
         <v>9820.227627208802</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>[-2.04477250e+08 -4.02385224e+07 -3.89206864e+07 -8.78982548e+08
  -1.23941045e+09]</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>[-0.09281113  0.00501875 -0.03231113 -0.1402273  -0.27067626]</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>[ -7657.71394167  -4773.9660222   -4228.52997215 -13363.10566351
  -19077.82253651]</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Dataset 1</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>SVR (RBF Kernel)</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>-0.08737487153970336</v>
-      </c>
-      <c r="D13" t="n">
-        <v>7003.501188517066</v>
-      </c>
-      <c r="E13" t="n">
-        <v>12584.07764949718</v>
-      </c>
-      <c r="F13" t="n">
-        <v>-0.1062014174225997</v>
-      </c>
-      <c r="G13" t="n">
-        <v>21918.16352119195</v>
-      </c>
-      <c r="H13" t="n">
-        <v>9820.227627208802</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>[-2.04477250e+08 -4.02385224e+07 -3.89206864e+07 -8.78982548e+08
- -1.23941045e+09]</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>[-0.09281113  0.00501875 -0.03231113 -0.1402273  -0.27067626]</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>[ -7657.71394167  -4773.9660222   -4228.52997215 -13363.10566351
- -19077.82253651]</t>
-        </is>
-      </c>
-    </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
@@ -1062,42 +1127,723 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>onehot</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>SVR (Sigmoid Kernel)</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>-0.08036218691983588</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>6964.719479724569</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>12543.43347378073</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>-0.1006732588117087</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>21889.68805299561</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>9794.523531732368</v>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>[-2.04145448e+08 -3.97724889e+07 -3.86078033e+07 -8.76080697e+08
  -1.23718578e+09]</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>[-0.09103784  0.01654239 -0.02401239 -0.13646298 -0.26839547]</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>[ -7642.83911925  -4746.31506427  -4212.31752338 -13319.68168976
  -19051.464262  ]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Regressao Linear</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.1793441791182908</v>
+      </c>
+      <c r="E15" t="n">
+        <v>7881.796727534091</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10932.31835981938</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-1.071502106997759</v>
+      </c>
+      <c r="H15" t="n">
+        <v>19767.79784084156</v>
+      </c>
+      <c r="I15" t="n">
+        <v>11966.18694274079</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>[-1.77321995e+08 -1.44358553e+08 -1.56867946e+08 -6.14316745e+08
+ -8.60963918e+08]</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>[ 0.0523178  -2.56956583 -3.16068014  0.20310053  0.1173171 ]</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>[ -9441.97226084  -8473.78207357 -10329.45107975 -14510.23178414
+ -17075.4975154 ]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Ridge</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.2230231644545568</v>
+      </c>
+      <c r="E16" t="n">
+        <v>7882.179212757857</v>
+      </c>
+      <c r="F16" t="n">
+        <v>10637.40706170515</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-1.070918593530145</v>
+      </c>
+      <c r="H16" t="n">
+        <v>19379.03658784059</v>
+      </c>
+      <c r="I16" t="n">
+        <v>11804.54454016315</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>[-1.70814114e+08 -1.36291958e+08 -1.69489678e+08 -5.13451658e+08
+ -8.87687887e+08]</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>[ 0.08709861 -2.37010246 -3.49545211  0.333944    0.08991898]</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>[ -9237.30079536  -8157.00373553 -10957.01500439 -12919.94737596
+ -17751.45578958]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Lasso</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.1798503143642369</v>
+      </c>
+      <c r="E17" t="n">
+        <v>7879.414542172697</v>
+      </c>
+      <c r="F17" t="n">
+        <v>10928.94661437372</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-1.070581424653915</v>
+      </c>
+      <c r="H17" t="n">
+        <v>19755.85107155388</v>
+      </c>
+      <c r="I17" t="n">
+        <v>11962.4296129948</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>[-1.77305126e+08 -1.44308307e+08 -1.56858350e+08 -6.11836845e+08
+ -8.61159629e+08]</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>[ 0.05240795 -2.56832339 -3.16042563  0.20631749  0.11711645]</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>[ -9442.20016894  -8472.58377175 -10332.32324201 -14492.66192141
+ -17072.37896086]</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ElasticNet</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.2359754165468076</v>
+      </c>
+      <c r="E18" t="n">
+        <v>7336.998857443184</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10548.37132637588</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-0.8586036765137587</v>
+      </c>
+      <c r="H18" t="n">
+        <v>19779.04011481213</v>
+      </c>
+      <c r="I18" t="n">
+        <v>11453.89266690852</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>[-1.55293837e+08 -9.48473634e+07 -1.65150651e+08 -5.80069792e+08
+ -9.60690496e+08]</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>[ 0.1700454  -1.34529856 -3.38036612  0.24752611  0.01507478]</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>[ -8370.12745717  -6656.77180131 -10639.6505096  -12713.39464602
+ -18889.51892044]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Arvore de Decisao</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.5063441948176337</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3797.957857142856</v>
+      </c>
+      <c r="F19" t="n">
+        <v>8478.985008420328</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-2.141421647532166</v>
+      </c>
+      <c r="H19" t="n">
+        <v>18601.76005442271</v>
+      </c>
+      <c r="I19" t="n">
+        <v>7955.690015789473</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>[-9.82575261e+08 -8.42119246e+06 -3.69775557e+08 -2.24969822e+08
+ -1.44385553e+08]</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>[-4.25128924  0.79176848 -8.8077259   0.7081663   0.85197213]</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>[-13546.119       -2162.204       -6538.2055      -9714.35736842
+  -7817.56421053]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.3364398029087947</v>
+      </c>
+      <c r="E20" t="n">
+        <v>7344.0557047619</v>
+      </c>
+      <c r="F20" t="n">
+        <v>13951.03550477201</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-0.9483667510981559</v>
+      </c>
+      <c r="H20" t="n">
+        <v>14730.45671902975</v>
+      </c>
+      <c r="I20" t="n">
+        <v>6778.367555105258</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>[-2.98209087e+08 -9.08638354e+06 -2.76761187e+08 -2.54525340e+08
+ -2.46349777e+08]</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>[-0.5937529   0.77532025 -6.34066332  0.6698265   0.74743572]</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>[-7674.88725    -2295.45164    -5946.562175   -8358.90164737
+ -9616.03506316]</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Gradient Boosting</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>-0.07565092407926532</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6495.82139300822</v>
+      </c>
+      <c r="F21" t="n">
+        <v>12516.05377663962</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-1.098920191617777</v>
+      </c>
+      <c r="H21" t="n">
+        <v>14033.75992326731</v>
+      </c>
+      <c r="I21" t="n">
+        <v>6489.434073618047</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>[-2.84375893e+08 -7.65295976e+06 -3.15478403e+08 -1.14801611e+08
+ -2.62423221e+08]</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>[-0.51982258  0.81076463 -7.36757771  0.8510779   0.7309568 ]</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>[ -6599.69333075  -2239.15570241  -6853.2380467   -6542.45944093
+ -10212.62384729]</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.3840503604608698</v>
+      </c>
+      <c r="E22" t="n">
+        <v>4483.48761441912</v>
+      </c>
+      <c r="F22" t="n">
+        <v>9471.185569398307</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-1.358780385582489</v>
+      </c>
+      <c r="H22" t="n">
+        <v>13882.34548512351</v>
+      </c>
+      <c r="I22" t="n">
+        <v>6615.869484757915</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>[-2.57935248e+08 -1.31018386e+07 -3.66423170e+08 -1.40614649e+08
+ -1.85522675e+08]</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>[-0.37851282  0.67602976 -8.71880903  0.8175929   0.80979726]</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>[-7118.43301685 -2715.17663953 -6551.84894037 -7759.36063986
+ -8934.52818719]</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>LightGBM</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>-0.221424720562138</v>
+      </c>
+      <c r="E23" t="n">
+        <v>9244.704704309386</v>
+      </c>
+      <c r="F23" t="n">
+        <v>13337.21327104575</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-0.6162352992704719</v>
+      </c>
+      <c r="H23" t="n">
+        <v>18603.13994849129</v>
+      </c>
+      <c r="I23" t="n">
+        <v>10767.88651626235</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>[-2.68957327e+08 -8.19447129e+07 -1.19554363e+08 -5.69136915e+08
+ -6.90790762e+08]</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>[-0.43741937 -1.02625366 -2.17099495  0.26170838  0.2917831 ]</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>[-10225.42836897  -6197.53710882  -8005.46944396 -13826.62474867
+ -15584.37291089]</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>CatBoost</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.3422212640109197</v>
+      </c>
+      <c r="E24" t="n">
+        <v>5271.35977412747</v>
+      </c>
+      <c r="F24" t="n">
+        <v>9787.497364321365</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.2949506147962433</v>
+      </c>
+      <c r="H24" t="n">
+        <v>10828.20358026546</v>
+      </c>
+      <c r="I24" t="n">
+        <v>5601.215213592752</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>[-9.19208325e+07 -1.24012758e+07 -8.61273568e+07 -1.36610705e+08
+ -2.59189794e+08]</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>[ 0.50873699  0.69335263 -1.2843952   0.82278686  0.73427179]</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>[-4552.33951582 -2604.53564337 -4254.73999135 -7748.52329999
+ -8845.93761743]</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>SVR (Linear Kernel)</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>-0.004669956856544921</v>
+      </c>
+      <c r="E25" t="n">
+        <v>6401.797175244348</v>
+      </c>
+      <c r="F25" t="n">
+        <v>12096.04658975622</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-0.07891610895017079</v>
+      </c>
+      <c r="H25" t="n">
+        <v>21777.67178506815</v>
+      </c>
+      <c r="I25" t="n">
+        <v>9524.896983813527</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>[-2.08255655e+08 -3.45142922e+07 -3.96870276e+07 -8.60074184e+08
+ -1.22880378e+09]</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>[-0.11300449  0.14656226 -0.05263715 -0.11569913 -0.25980202]</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>[ -7347.64219923  -4142.74045595  -4105.91700643 -13022.72298743
+ -19005.46227002]</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>SVR (RBF Kernel)</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>-0.08837499942213611</v>
+      </c>
+      <c r="E26" t="n">
+        <v>7020.831846484198</v>
+      </c>
+      <c r="F26" t="n">
+        <v>12589.86350800241</v>
+      </c>
+      <c r="G26" t="n">
+        <v>-0.1079539275646776</v>
+      </c>
+      <c r="H26" t="n">
+        <v>21911.00959004555</v>
+      </c>
+      <c r="I26" t="n">
+        <v>9818.659239470415</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>[-2.04762804e+08 -4.03674508e+07 -3.91542982e+07 -8.79438312e+08
+ -1.23673884e+09]</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>[-0.09433725  0.00183072 -0.03850733 -0.14081852 -0.26793726]</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>[ -7659.15175107  -4768.43299282  -4222.42677213 -13371.56783695
+ -19071.71684439]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>SVR (Sigmoid Kernel)</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>-0.09101652355645018</v>
+      </c>
+      <c r="E27" t="n">
+        <v>7025.543332458004</v>
+      </c>
+      <c r="F27" t="n">
+        <v>12605.13226837616</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-0.1097108296855151</v>
+      </c>
+      <c r="H27" t="n">
+        <v>21925.73538015443</v>
+      </c>
+      <c r="I27" t="n">
+        <v>9830.934588235679</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>[-2.04924257e+08 -4.04818357e+07 -3.92261461e+07 -8.80302196e+08
+ -1.23875492e+09]</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>[-0.09520012 -0.00099768 -0.04041298 -0.14193917 -0.2700042 ]</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>[ -7667.43979455  -4786.52320417  -4234.73977455 -13381.79287811
+ -19084.17728978]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Run regression models with the original dataset (few changes)
</commit_message>
<xml_diff>
--- a/Jupyter/Python/resultados_regressao.xlsx
+++ b/Jupyter/Python/resultados_regressao.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,38 +512,38 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>-1.191779160026281</v>
+        <v>0.3637007023772486</v>
       </c>
       <c r="E2" t="n">
-        <v>9747.457259750538</v>
+        <v>1359.403337559624</v>
       </c>
       <c r="F2" t="n">
-        <v>17866.11560270452</v>
+        <v>2443.518208291927</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.4551661381186431</v>
+        <v>0.2450165869887393</v>
       </c>
       <c r="H2" t="n">
-        <v>20544.39727538676</v>
+        <v>2816.742949764204</v>
       </c>
       <c r="I2" t="n">
-        <v>10278.90184040628</v>
+        <v>1527.504056685391</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[-5.36936080e+08 -4.84330921e+07 -6.09596707e+07 -3.33792368e+08
- -1.13024009e+09]</t>
+          <t>[-10857417.46080197 -10172348.84330518  -7108460.70785512
+  -4699413.02711611  -6832564.18615337]</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[-1.86960885 -0.19760905 -0.61686118  0.56700031 -0.15875193]</t>
+          <t>[0.39213972 0.25404521 0.07722352 0.20773125 0.29394324]</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[ -9896.10240574  -6241.48377845  -5617.34012575 -11961.72481999
- -17677.85807211]</t>
+          <t>[-1704.89357022 -1570.26079203 -1568.95720887 -1385.14718872
+ -1408.26152358]</t>
         </is>
       </c>
     </row>
@@ -564,38 +564,38 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-0.7811135038951063</v>
+        <v>0.3465656542175181</v>
       </c>
       <c r="E3" t="n">
-        <v>8855.464493685831</v>
+        <v>1350.756121257281</v>
       </c>
       <c r="F3" t="n">
-        <v>16105.62345992551</v>
+        <v>2476.200669748001</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.07832636867183637</v>
+        <v>0.2708386209746564</v>
       </c>
       <c r="H3" t="n">
-        <v>17290.32346778754</v>
+        <v>2779.530533181231</v>
       </c>
       <c r="I3" t="n">
-        <v>8779.115747629901</v>
+        <v>1473.301915964293</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[-3.76445292e+08 -3.31225718e+07 -5.31547431e+07 -3.41162024e+08
- -6.90891797e+08]</t>
+          <t>[-10983800.36198915  -9800036.22126423  -6655489.99357756
+  -4474073.35081207  -6715549.99679071]</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>[-1.01187959  0.18097544 -0.40984752  0.5574403   0.29167952]</t>
+          <t>[0.38506408 0.28134749 0.13602538 0.24572101 0.30603514]</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[ -8565.76416386  -4887.84968104  -5681.0247185  -11750.18556298
- -13010.75461177]</t>
+          <t>[-1635.17180963 -1530.64350962 -1503.94778329 -1340.98331259
+ -1355.76316469]</t>
         </is>
       </c>
     </row>
@@ -616,38 +616,38 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>-1.189103663936121</v>
+        <v>0.3631380827872364</v>
       </c>
       <c r="E4" t="n">
-        <v>9732.808719593968</v>
+        <v>1293.778358927309</v>
       </c>
       <c r="F4" t="n">
-        <v>17855.20772481208</v>
+        <v>2444.598256200787</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.38354761714424</v>
+        <v>0.2627666365996696</v>
       </c>
       <c r="H4" t="n">
-        <v>19943.25743860208</v>
+        <v>2787.333508619871</v>
       </c>
       <c r="I4" t="n">
-        <v>9807.728526960354</v>
+        <v>1426.829463415926</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>[-4.94040160e+08 -4.77261766e+07 -6.05320644e+07 -2.58806791e+08
- -1.12756239e+09]</t>
+          <t>[-10648691.1543616  -10039465.57238786  -6874489.81407488
+  -4526700.23302349  -6756793.66752796]</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>[-1.64035528 -0.1801291  -0.60551958  0.66427255 -0.15600669]</t>
+          <t>[0.40382541 0.26378975 0.10759618 0.2368487  0.30177314]</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[ -8529.24449514  -6181.36508366  -5601.86556906 -11103.01550649
- -17623.15198045]</t>
+          <t>[-1597.85085581 -1468.25599283 -1473.66340717 -1293.82267797
+ -1300.55438331]</t>
         </is>
       </c>
     </row>
@@ -668,38 +668,38 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.342469142165772</v>
+        <v>0.09136184800287006</v>
       </c>
       <c r="E5" t="n">
-        <v>7397.197215428671</v>
+        <v>1362.646682834279</v>
       </c>
       <c r="F5" t="n">
-        <v>9785.653024225001</v>
+        <v>2919.983125682414</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.001095598073094162</v>
+        <v>0.1026980304295909</v>
       </c>
       <c r="H5" t="n">
-        <v>18691.39407988569</v>
+        <v>3145.84684173973</v>
       </c>
       <c r="I5" t="n">
-        <v>10303.0258197788</v>
+        <v>1441.700279301547</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>[-1.43475822e+08 -3.80155820e+07 -6.04523021e+07 -5.60340303e+08
- -9.44557054e+08]</t>
+          <t>[-16377563.21184384 -12443846.26276871  -6993736.38796142
+  -5163407.71147194  -8503208.18437326]</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>[ 0.23320577  0.05998558 -0.60340401  0.27311946  0.03161521]</t>
+          <t>[0.08309041 0.08747263 0.09211632 0.12950691 0.12130389]</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[ -8349.24679487  -5397.95820809  -7216.00015016 -12770.67073553
- -17781.25321025]</t>
+          <t>[-1704.55023045 -1520.90309057 -1374.77977156 -1235.60858414
+ -1372.65971978]</t>
         </is>
       </c>
     </row>
@@ -720,38 +720,38 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.1902533389644809</v>
+        <v>0.4826255469141713</v>
       </c>
       <c r="E6" t="n">
-        <v>5341.505476190476</v>
+        <v>811.6219756961431</v>
       </c>
       <c r="F6" t="n">
-        <v>10859.41239407207</v>
+        <v>2203.369573003884</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3410851386779976</v>
+        <v>-0.2385748807143094</v>
       </c>
       <c r="H6" t="n">
-        <v>16353.68763897397</v>
+        <v>3534.49009913668</v>
       </c>
       <c r="I6" t="n">
-        <v>7251.092378947369</v>
+        <v>1143.509060522626</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>[-1.46487313e+08 -2.11219306e+07 -2.59618498e+07 -4.71749195e+08
- -6.71895209e+08]</t>
+          <t>[-18281414.52062094 -13185449.19614461  -8476551.19174238
+ -11876678.5289201  -10643007.86704805]</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>[0.21711111 0.47771628 0.31140201 0.38804097 0.31115532]</t>
+          <t>[-0.02349807  0.03308969 -0.10037354 -1.00227587 -0.09981661]</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[ -5674.2225      -3103.968       -3192.9135     -11036.85526316
- -13247.50263158]</t>
+          <t>[-1468.65996601 -1102.01001571 -1071.47609226 -1092.3105023
+  -983.08872633]</t>
         </is>
       </c>
     </row>
@@ -772,38 +772,38 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-0.2128334802360237</v>
+        <v>0.4997038994942687</v>
       </c>
       <c r="E7" t="n">
-        <v>6786.339497619042</v>
+        <v>845.6365655948883</v>
       </c>
       <c r="F7" t="n">
-        <v>13290.22494555015</v>
+        <v>2166.69817038607</v>
       </c>
       <c r="G7" t="n">
-        <v>0.344922087615741</v>
+        <v>0.1874750160486846</v>
       </c>
       <c r="H7" t="n">
-        <v>14918.77776147562</v>
+        <v>2891.796115706427</v>
       </c>
       <c r="I7" t="n">
-        <v>6402.480938157893</v>
+        <v>1009.339525010073</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>[-3.14597134e+08 -8.58957120e+06 -1.92263023e+07 -3.00887103e+08
- -4.69549539e+08]</t>
+          <t>[-11515106.7608824  -10079226.79403951  -7619570.38083548
+  -5943101.64116601  -6655418.29715049]</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>[-0.68133741  0.78760497  0.49005201  0.60968544  0.51860544]</t>
+          <t>[ 0.35531851  0.260874    0.01087442 -0.00194082  0.31224897]</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>[ -7387.206105    -2065.758205    -2802.203865    -8930.18904737
- -10827.04746842]</t>
+          <t>[-1253.22645945 -1031.47333957  -956.7228708   -902.80966494
+  -902.46529031]</t>
         </is>
       </c>
     </row>
@@ -824,38 +824,39 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.415519116077802</v>
+        <v>0.4623771576710093</v>
       </c>
       <c r="E8" t="n">
-        <v>4631.970034285237</v>
+        <v>1068.957886968166</v>
       </c>
       <c r="F8" t="n">
-        <v>9226.073263353755</v>
+        <v>2246.072207348774</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2470576331221443</v>
+        <v>0.2047516159873858</v>
       </c>
       <c r="H8" t="n">
-        <v>16070.29642638487</v>
+        <v>2874.678853763635</v>
       </c>
       <c r="I8" t="n">
-        <v>6924.740470993594</v>
+        <v>1189.555803537321</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>[-3.42753814e+08 -6.49125207e+06 -2.81805786e+07 -3.23684957e+08
- -5.90161535e+08]</t>
+          <t>[-11550725.4102504   -9688741.38954905  -7700954.21494526
+  -5214113.84002944  -7164357.70660487]</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>[-0.83181837  0.83949028  0.25255365  0.58011177  0.39495084]</t>
+          <t>[3.53324375e-01 2.89508925e-01 3.09669678e-04 1.20958416e-01
+ 2.59656694e-01]</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>[ -7224.71615991  -1968.30782832  -3138.92935799  -9450.7585784
- -12840.99043035]</t>
+          <t>[-1423.25148946 -1188.75314377 -1182.88999231 -1055.87151683
+ -1097.01287532]</t>
         </is>
       </c>
     </row>
@@ -876,38 +877,38 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.6258352068970525</v>
+        <v>0.4773345836526366</v>
       </c>
       <c r="E9" t="n">
-        <v>3682.10621673584</v>
+        <v>921.2469383090279</v>
       </c>
       <c r="F9" t="n">
-        <v>7381.815788899872</v>
+        <v>2214.607365708936</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4363103065024265</v>
+        <v>0.2946508710906291</v>
       </c>
       <c r="H9" t="n">
-        <v>14264.41864593009</v>
+        <v>2624.029528414364</v>
       </c>
       <c r="I9" t="n">
-        <v>6212.615042119718</v>
+        <v>1002.502499629306</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>[-1.83873811e+08 -8.04407659e+06 -2.79335274e+07 -2.87937945e+08
- -5.09578837e+08]</t>
+          <t>[-8838189.24250673 -8056866.26743571 -6570182.54580689 -6978901.84682448
+ -3983514.92737873]</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>[0.01730218 0.80109346 0.2591063  0.62648325 0.47756635]</t>
+          <t>[ 0.50518765  0.40917697  0.14709947 -0.17656521  0.58835548]</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>[ -5267.67803333  -1951.45250012  -3407.60198984  -9521.21791838
- -10915.12476893]</t>
+          <t>[-1195.35197686 -1043.8656782   -950.25943271  -989.23881708
+  -833.7965933 ]</t>
         </is>
       </c>
     </row>
@@ -928,38 +929,38 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-0.5062336308909425</v>
+        <v>0.5449233305295333</v>
       </c>
       <c r="E10" t="n">
-        <v>9402.940989458264</v>
+        <v>987.7141120111936</v>
       </c>
       <c r="F10" t="n">
-        <v>14810.77939627252</v>
+        <v>2066.460666207457</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.7411596952515552</v>
+        <v>0.3168509829689449</v>
       </c>
       <c r="H10" t="n">
-        <v>19530.44383360109</v>
+        <v>2690.267657475169</v>
       </c>
       <c r="I10" t="n">
-        <v>10822.51912859489</v>
+        <v>1169.61798212249</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>[-2.76605469e+08 -5.80258760e+07 -1.58249892e+08 -5.34481653e+08
- -8.79828292e+08]</t>
+          <t>[-10576542.63346839  -9299341.37745446  -6960042.72255747
+  -4165090.76245168  -5186682.84835267]</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>[-0.47829421 -0.43481061 -3.19733412  0.30666363  0.09797685]</t>
+          <t>[0.40786469 0.31806426 0.09649023 0.29781204 0.4640237 ]</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[-10018.5647826   -5643.43607803  -9006.64071117 -11911.40488544
- -17532.54918574]</t>
+          <t>[-1372.07297635 -1259.93761492 -1154.98764454 -1005.60182584
+ -1055.48984896]</t>
         </is>
       </c>
     </row>
@@ -980,38 +981,38 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.4032481595475715</v>
+        <v>0.5860936844489558</v>
       </c>
       <c r="E11" t="n">
-        <v>4812.576743866931</v>
+        <v>899.9137651643006</v>
       </c>
       <c r="F11" t="n">
-        <v>9322.419174141065</v>
+        <v>1970.769735014384</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3522514500934445</v>
+        <v>0.4137877476540349</v>
       </c>
       <c r="H11" t="n">
-        <v>14858.62242451191</v>
+        <v>2428.832435701565</v>
       </c>
       <c r="I11" t="n">
-        <v>6530.750213051405</v>
+        <v>994.4156939837679</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>[-2.70000843e+08 -1.13316167e+07 -2.45974495e+07 -1.65618951e+08
- -6.32344441e+08]</t>
+          <t>[-7292254.02055366 -7118757.38861865 -6042588.93326105 -4320629.4531068
+ -4721905.20803983]</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>[-0.44299636  0.71980218  0.34759062  0.785157    0.35170381]</t>
+          <t>[0.59173794 0.47797001 0.21558841 0.27158994 0.51205243]</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>[ -5841.93850766  -2563.5335398   -3167.97967961  -8365.2116056
- -12715.08773258]</t>
+          <t>[-1118.04667078 -1035.41890816  -995.94759485  -927.89744218
+  -894.76785395]</t>
         </is>
       </c>
     </row>
@@ -1032,38 +1033,38 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>-0.03328874256371361</v>
+        <v>-0.005796476814591722</v>
       </c>
       <c r="E12" t="n">
-        <v>6629.315706845121</v>
+        <v>978.6295743306747</v>
       </c>
       <c r="F12" t="n">
-        <v>12267.11939030785</v>
+        <v>3072.132287395591</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.06225202916850434</v>
+        <v>-0.005167692482741892</v>
       </c>
       <c r="H12" t="n">
-        <v>21703.08592950889</v>
+        <v>3325.302883096542</v>
       </c>
       <c r="I12" t="n">
-        <v>9565.182123314622</v>
+        <v>1056.989268857788</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>[-2.03477029e+08 -3.58466103e+07 -3.67546654e+07 -8.49541734e+08
- -1.22949965e+09]</t>
+          <t>[-18133744.41149002 -13827090.37165851  -7787913.88376387
+  -5821534.07822253  -9717913.57651595]</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>[-0.08746554  0.11361792  0.02513923 -0.1020363  -0.26051545]</t>
+          <t>[-0.01523065 -0.0139629  -0.0109789   0.01855412 -0.00422014]</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>[ -7477.32311968  -4481.13756644  -4034.60548982 -12960.55953361
- -18872.28490702]</t>
+          <t>[-1357.47525427 -1135.33868612  -972.75789519  -815.33457383
+ -1004.03993488]</t>
         </is>
       </c>
     </row>
@@ -1084,38 +1085,38 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>-0.08737487153970336</v>
+        <v>-0.0698329142205294</v>
       </c>
       <c r="E13" t="n">
-        <v>7003.501188517066</v>
+        <v>1027.742675270381</v>
       </c>
       <c r="F13" t="n">
-        <v>12584.07764949718</v>
+        <v>3168.420651021299</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.1062014174225997</v>
+        <v>-0.07952577207297748</v>
       </c>
       <c r="H13" t="n">
-        <v>21918.16352119195</v>
+        <v>3437.87387231447</v>
       </c>
       <c r="I13" t="n">
-        <v>9820.227627208802</v>
+        <v>1121.071921693741</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>[-2.04477250e+08 -4.02385224e+07 -3.89206864e+07 -8.78982548e+08
- -1.23941045e+09]</t>
+          <t>[-19282802.59268318 -14570319.93075719  -8398390.39360878
+  -6418689.54911447 -10424681.34354883]</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>[-0.09281113  0.00501875 -0.03231113 -0.1402273  -0.27067626]</t>
+          <t>[-0.0795615  -0.06846512 -0.09022719 -0.08211965 -0.0772554 ]</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>[ -7657.71394167  -4773.9660222   -4228.52997215 -13363.10566351
- -19077.82253651]</t>
+          <t>[-1424.5206359  -1191.6169954  -1022.38586862  -885.5825174
+ -1081.25359116]</t>
         </is>
       </c>
     </row>
@@ -1136,38 +1137,38 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>-0.08036218691983588</v>
+        <v>-0.06987497509720475</v>
       </c>
       <c r="E14" t="n">
-        <v>6964.719479724569</v>
+        <v>1032.424296885026</v>
       </c>
       <c r="F14" t="n">
-        <v>12543.43347378073</v>
+        <v>3168.482934223964</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.1006732588117087</v>
+        <v>-0.0775690133805694</v>
       </c>
       <c r="H14" t="n">
-        <v>21889.68805299561</v>
+        <v>3434.907945998368</v>
       </c>
       <c r="I14" t="n">
-        <v>9794.523531732368</v>
+        <v>1124.519892343182</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>[-2.04145448e+08 -3.97724889e+07 -3.86078033e+07 -8.76080697e+08
- -1.23718578e+09]</t>
+          <t>[-19249360.85240111 -14546679.04969465  -8390955.7287757
+  -6398036.99303116 -10407930.36351102]</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>[-0.09103784  0.01654239 -0.02401239 -0.13646298 -0.26839547]</t>
+          <t>[-0.07768924 -0.0667315  -0.08926207 -0.07863786 -0.07552441]</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>[ -7642.83911925  -4746.31506427  -4212.31752338 -13319.68168976
- -19051.464262  ]</t>
+          <t>[-1431.56731532 -1196.07184004 -1024.38821394  -888.36779867
+ -1082.20429375]</t>
         </is>
       </c>
     </row>
@@ -1188,38 +1189,38 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.1793441791182908</v>
+        <v>0.06655306872829769</v>
       </c>
       <c r="E15" t="n">
-        <v>7881.796727534091</v>
+        <v>1424.041516858642</v>
       </c>
       <c r="F15" t="n">
-        <v>10932.31835981938</v>
+        <v>2959.577205969633</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.071502106997759</v>
+        <v>0.07520618207100864</v>
       </c>
       <c r="H15" t="n">
-        <v>19767.79784084156</v>
+        <v>3175.458220696377</v>
       </c>
       <c r="I15" t="n">
-        <v>11966.18694274079</v>
+        <v>1553.996549923185</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>[-1.77321995e+08 -1.44358553e+08 -1.56867946e+08 -6.14316745e+08
- -8.60963918e+08]</t>
+          <t>[-16160364.79484257 -12688008.14773007  -7411864.73010133
+  -5572831.28292792  -8584605.60133912]</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>[ 0.0523178  -2.56956583 -3.16068014  0.20310053  0.1173171 ]</t>
+          <t>[0.09525042 0.06956784 0.03783748 0.06048265 0.11289252]</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>[ -9441.97226084  -8473.78207357 -10329.45107975 -14510.23178414
- -17075.4975154 ]</t>
+          <t>[-1817.6831608  -1662.57400273 -1451.95980014 -1376.16699901
+ -1461.59878695]</t>
         </is>
       </c>
     </row>
@@ -1240,38 +1241,38 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.2230231644545568</v>
+        <v>0.06654667560720873</v>
       </c>
       <c r="E16" t="n">
-        <v>7882.179212757857</v>
+        <v>1424.024193840323</v>
       </c>
       <c r="F16" t="n">
-        <v>10637.40706170515</v>
+        <v>2959.587340934149</v>
       </c>
       <c r="G16" t="n">
-        <v>-1.070918593530145</v>
+        <v>0.07529546273327237</v>
       </c>
       <c r="H16" t="n">
-        <v>19379.03658784059</v>
+        <v>3175.343934299048</v>
       </c>
       <c r="I16" t="n">
-        <v>11804.54454016315</v>
+        <v>1553.865769154645</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>[-1.70814114e+08 -1.36291958e+08 -1.69489678e+08 -5.13451658e+08
- -8.87687887e+08]</t>
+          <t>[-16160299.48646909 -12688056.66825351  -7409487.29968724
+  -5572676.83903785  -8583525.21200108]</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>[ 0.08709861 -2.37010246 -3.49545211  0.333944    0.08991898]</t>
+          <t>[0.09525407 0.06956428 0.03814611 0.06050868 0.11300417]</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>[ -9237.30079536  -8157.00373553 -10957.01500439 -12919.94737596
- -17751.45578958]</t>
+          <t>[-1817.66397245 -1662.5734949  -1451.79909625 -1376.12228349
+ -1461.16999869]</t>
         </is>
       </c>
     </row>
@@ -1292,38 +1293,38 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.1798503143642369</v>
+        <v>0.06650180523069849</v>
       </c>
       <c r="E17" t="n">
-        <v>7879.414542172697</v>
+        <v>1423.908709982711</v>
       </c>
       <c r="F17" t="n">
-        <v>10928.94661437372</v>
+        <v>2959.65847261208</v>
       </c>
       <c r="G17" t="n">
-        <v>-1.070581424653915</v>
+        <v>0.07550486069966582</v>
       </c>
       <c r="H17" t="n">
-        <v>19755.85107155388</v>
+        <v>3175.040508851472</v>
       </c>
       <c r="I17" t="n">
-        <v>11962.4296129948</v>
+        <v>1553.397766627049</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>[-1.77305126e+08 -1.44308307e+08 -1.56858350e+08 -6.11836845e+08
- -8.61159629e+08]</t>
+          <t>[-16157880.16086774 -12688144.84279202  -7406410.60131279
+  -5571422.35950772  -8580553.1997588 ]</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>[ 0.05240795 -2.56832339 -3.16042563  0.20631749  0.11711645]</t>
+          <t>[0.09538952 0.06955782 0.0385455  0.06072018 0.11331129]</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>[ -9442.20016894  -8472.58377175 -10332.32324201 -14492.66192141
- -17072.37896086]</t>
+          <t>[-1817.33572389 -1662.29067796 -1451.57969766 -1375.79200419
+ -1459.99072944]</t>
         </is>
       </c>
     </row>
@@ -1344,38 +1345,38 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.2359754165468076</v>
+        <v>0.06292223943575692</v>
       </c>
       <c r="E18" t="n">
-        <v>7336.998857443184</v>
+        <v>1426.45261778661</v>
       </c>
       <c r="F18" t="n">
-        <v>10548.37132637588</v>
+        <v>2965.32755455293</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.8586036765137587</v>
+        <v>0.08016718330429869</v>
       </c>
       <c r="H18" t="n">
-        <v>19779.04011481213</v>
+        <v>3171.251664362963</v>
       </c>
       <c r="I18" t="n">
-        <v>11453.89266690852</v>
+        <v>1545.004345211573</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>[-1.55293837e+08 -9.48473634e+07 -1.65150651e+08 -5.80069792e+08
- -9.60690496e+08]</t>
+          <t>[-16250588.04274295 -12714902.88302004  -7297529.32800926
+  -5528323.07251891  -8492842.26733317]</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>[ 0.1700454  -1.34529856 -3.38036612  0.24752611  0.01507478]</t>
+          <t>[0.0901992  0.06759561 0.0526798  0.06798624 0.12237507]</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>[ -8370.12745717  -6656.77180131 -10639.6505096  -12713.39464602
- -18889.51892044]</t>
+          <t>[-1817.61036476 -1666.03851043 -1450.96653081 -1364.39151906
+ -1426.01480099]</t>
         </is>
       </c>
     </row>
@@ -1396,38 +1397,38 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.5063441948176337</v>
+        <v>0.4336801275175118</v>
       </c>
       <c r="E19" t="n">
-        <v>3797.957857142856</v>
+        <v>887.3224699676803</v>
       </c>
       <c r="F19" t="n">
-        <v>8478.985008420328</v>
+        <v>2305.237938828828</v>
       </c>
       <c r="G19" t="n">
-        <v>-2.141421647532166</v>
+        <v>0.1828842738328417</v>
       </c>
       <c r="H19" t="n">
-        <v>18601.76005442271</v>
+        <v>2801.418144033501</v>
       </c>
       <c r="I19" t="n">
-        <v>7955.690015789473</v>
+        <v>1071.381957769768</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>[-9.82575261e+08 -8.42119246e+06 -3.69775557e+08 -2.24969822e+08
- -1.44385553e+08]</t>
+          <t>[-8498262.46497982 -8561703.05144286 -6144302.42489115 -8080733.33153399
+ -7954716.8157527 ]</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>[-4.25128924  0.79176848 -8.8077259   0.7081663   0.85197213]</t>
+          <t>[ 0.5242187   0.37215647  0.20238459 -0.36232174  0.17798335]</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>[-13546.119       -2162.204       -6538.2055      -9714.35736842
-  -7817.56421053]</t>
+          <t>[-1098.73668398 -1042.1926898   -945.17186856 -1177.60166413
+ -1093.20688237]</t>
         </is>
       </c>
     </row>
@@ -1448,38 +1449,38 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>-0.3364398029087947</v>
+        <v>0.6058071486892533</v>
       </c>
       <c r="E20" t="n">
-        <v>7344.0557047619</v>
+        <v>835.897822570838</v>
       </c>
       <c r="F20" t="n">
-        <v>13951.03550477201</v>
+        <v>1923.265449168233</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.9483667510981559</v>
+        <v>0.4348691734847274</v>
       </c>
       <c r="H20" t="n">
-        <v>14730.45671902975</v>
+        <v>2392.244558490173</v>
       </c>
       <c r="I20" t="n">
-        <v>6778.367555105258</v>
+        <v>1011.591359907379</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>[-2.98209087e+08 -9.08638354e+06 -2.76761187e+08 -2.54525340e+08
- -2.46349777e+08]</t>
+          <t>[-7917790.79245546 -5893293.8106124  -6114815.28433993 -3963085.9408158
+ -4725184.30990563]</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>[-0.5937529   0.77532025 -6.34066332  0.6698265   0.74743572]</t>
+          <t>[0.55671682 0.56783523 0.20621243 0.3318678  0.51171358]</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>[-7674.88725    -2295.45164    -5946.562175   -8358.90164737
- -9616.03506316]</t>
+          <t>[-1183.84999656  -948.93694704 -1028.97938704  -961.14246474
+  -935.04800415]</t>
         </is>
       </c>
     </row>
@@ -1500,38 +1501,38 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>-0.07565092407926532</v>
+        <v>0.27638028821252</v>
       </c>
       <c r="E21" t="n">
-        <v>6495.82139300822</v>
+        <v>1179.144847705463</v>
       </c>
       <c r="F21" t="n">
-        <v>12516.05377663962</v>
+        <v>2605.793833789446</v>
       </c>
       <c r="G21" t="n">
-        <v>-1.098920191617777</v>
+        <v>0.2489936446607239</v>
       </c>
       <c r="H21" t="n">
-        <v>14033.75992326731</v>
+        <v>2806.837151509023</v>
       </c>
       <c r="I21" t="n">
-        <v>6489.434073618047</v>
+        <v>1250.833622260753</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>[-2.84375893e+08 -7.65295976e+06 -3.15478403e+08 -1.14801611e+08
- -2.62423221e+08]</t>
+          <t>[-11519690.39703216  -8962989.92203514  -7253496.60583008
+  -4701394.54227064  -6954102.50828841]</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>[-0.51982258  0.81076463 -7.36757771  0.8510779   0.7309568 ]</t>
+          <t>[0.35506189 0.34272945 0.05839585 0.20739719 0.28138384]</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>[ -6599.69333075  -2239.15570241  -6853.2380467   -6542.45944093
- -10212.62384729]</t>
+          <t>[-1438.87832456 -1265.94977611 -1272.32013131 -1117.4812266
+ -1159.53865274]</t>
         </is>
       </c>
     </row>
@@ -1552,38 +1553,38 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.3840503604608698</v>
+        <v>0.5126461737097376</v>
       </c>
       <c r="E22" t="n">
-        <v>4483.48761441912</v>
+        <v>946.713077166178</v>
       </c>
       <c r="F22" t="n">
-        <v>9471.185569398307</v>
+        <v>2138.489133303085</v>
       </c>
       <c r="G22" t="n">
-        <v>-1.358780385582489</v>
+        <v>0.315874333234914</v>
       </c>
       <c r="H22" t="n">
-        <v>13882.34548512351</v>
+        <v>2594.947351862484</v>
       </c>
       <c r="I22" t="n">
-        <v>6615.869484757915</v>
+        <v>1095.594982754393</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>[-2.57935248e+08 -1.31018386e+07 -3.66423170e+08 -1.40614649e+08
- -1.85522675e+08]</t>
+          <t>[-10056434.67913384  -5687315.50722141  -7550463.41869108
+  -5951133.78120043  -4423411.40844384]</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>[-0.37851282  0.67602976 -8.71880903  0.8175929   0.80979726]</t>
+          <t>[ 0.43698331  0.58293996  0.01984546 -0.00329495  0.54289789]</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>[-7118.43301685 -2715.17663953 -6551.84894037 -7759.36063986
- -8934.52818719]</t>
+          <t>[-1252.23816093 -1025.99255181 -1140.47936886 -1091.23862008
+  -968.02621208]</t>
         </is>
       </c>
     </row>
@@ -1604,38 +1605,38 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>-0.221424720562138</v>
+        <v>0.565733421028016</v>
       </c>
       <c r="E23" t="n">
-        <v>9244.704704309386</v>
+        <v>937.2988714345378</v>
       </c>
       <c r="F23" t="n">
-        <v>13337.21327104575</v>
+        <v>2018.659460365097</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.6162352992704719</v>
+        <v>0.4187644195374382</v>
       </c>
       <c r="H23" t="n">
-        <v>18603.13994849129</v>
+        <v>2469.115319013638</v>
       </c>
       <c r="I23" t="n">
-        <v>10767.88651626235</v>
+        <v>1107.434869049275</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>[-2.68957327e+08 -8.19447129e+07 -1.19554363e+08 -5.69136915e+08
- -6.90790762e+08]</t>
+          <t>[-9405255.16624845 -6632022.42249031 -5933764.25186838 -3730652.29804315
+ -4780958.15428881]</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>[-0.43741937 -1.02625366 -2.17099495  0.26170838  0.2917831 ]</t>
+          <t>[0.47344006 0.51366307 0.22971536 0.37105353 0.50595008]</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>[-10225.42836897  -6197.53710882  -8005.46944396 -13826.62474867
- -15584.37291089]</t>
+          <t>[-1286.35620523 -1103.06472113 -1135.6314599   -994.33301287
+ -1017.78894612]</t>
         </is>
       </c>
     </row>
@@ -1656,38 +1657,38 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.3422212640109197</v>
+        <v>0.6065377467238257</v>
       </c>
       <c r="E24" t="n">
-        <v>5271.35977412747</v>
+        <v>895.0657820448289</v>
       </c>
       <c r="F24" t="n">
-        <v>9787.497364321365</v>
+        <v>1921.482330034781</v>
       </c>
       <c r="G24" t="n">
-        <v>0.2949506147962433</v>
+        <v>0.4653793257810525</v>
       </c>
       <c r="H24" t="n">
-        <v>10828.20358026546</v>
+        <v>2341.183009587624</v>
       </c>
       <c r="I24" t="n">
-        <v>5601.215213592752</v>
+        <v>1002.189111812718</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>[-9.19208325e+07 -1.24012758e+07 -8.61273568e+07 -1.36610705e+08
- -2.59189794e+08]</t>
+          <t>[-7473736.59598244 -6400244.19773829 -5640273.17988046 -3642468.14214725
+ -4248967.30616039]</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>[ 0.50873699  0.69335263 -1.2843952   0.82278686  0.73427179]</t>
+          <t>[0.58157751 0.53065974 0.26781456 0.3859204  0.56092442]</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>[-4552.33951582 -2604.53564337 -4254.73999135 -7748.52329999
- -8845.93761743]</t>
+          <t>[-1111.47215525 -1046.98385681 -1009.49108907  -916.95340535
+  -926.04505258]</t>
         </is>
       </c>
     </row>
@@ -1708,38 +1709,38 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>-0.004669956856544921</v>
+        <v>-0.04176844789775203</v>
       </c>
       <c r="E25" t="n">
-        <v>6401.797175244348</v>
+        <v>1036.089348917875</v>
       </c>
       <c r="F25" t="n">
-        <v>12096.04658975622</v>
+        <v>3126.586566355648</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.07891610895017079</v>
+        <v>-0.04624461709653369</v>
       </c>
       <c r="H25" t="n">
-        <v>21777.67178506815</v>
+        <v>3387.40374127831</v>
       </c>
       <c r="I25" t="n">
-        <v>9524.896983813527</v>
+        <v>1117.037599374863</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>[-2.08255655e+08 -3.45142922e+07 -3.96870276e+07 -8.60074184e+08
- -1.22880378e+09]</t>
+          <t>[-18708945.1466581  -14286995.15561561  -8214555.84653381
+  -6124005.0311227  -10038019.35220123]</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>[-0.11300449  0.14656226 -0.05263715 -0.11569913 -0.25980202]</t>
+          <t>[-0.04743368 -0.04768846 -0.06636292 -0.03243912 -0.03729891]</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>[ -7347.64219923  -4142.74045595  -4105.91700643 -13022.72298743
- -19005.46227002]</t>
+          <t>[-1429.40378895 -1188.66639033 -1027.85503059  -881.57218867
+ -1057.69059833]</t>
         </is>
       </c>
     </row>
@@ -1760,38 +1761,38 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>-0.08837499942213611</v>
+        <v>-0.06903327820549299</v>
       </c>
       <c r="E26" t="n">
-        <v>7020.831846484198</v>
+        <v>1047.295952902495</v>
       </c>
       <c r="F26" t="n">
-        <v>12589.86350800241</v>
+        <v>3167.236327360988</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.1079539275646776</v>
+        <v>-0.07686134571251549</v>
       </c>
       <c r="H26" t="n">
-        <v>21911.00959004555</v>
+        <v>3434.574539961992</v>
       </c>
       <c r="I26" t="n">
-        <v>9818.659239470415</v>
+        <v>1136.762655943043</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>[-2.04762804e+08 -4.03674508e+07 -3.91542982e+07 -8.79438312e+08
- -1.23673884e+09]</t>
+          <t>[-19274928.96411454 -14561019.94033882  -8327808.63228582
+  -6412717.96271793 -10405035.85331855]</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>[-0.09433725  0.00183072 -0.03850733 -0.14081852 -0.26793726]</t>
+          <t>[-0.07912069 -0.06778314 -0.0810647  -0.0811129  -0.0752253 ]</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>[ -7659.15175107  -4768.43299282  -4222.42677213 -13371.56783695
- -19071.71684439]</t>
+          <t>[-1448.3072123  -1202.6684692  -1031.25689554  -906.50866431
+ -1095.07203837]</t>
         </is>
       </c>
     </row>
@@ -1812,38 +1813,714 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>-0.09101652355645018</v>
+        <v>-0.08787207612756953</v>
       </c>
       <c r="E27" t="n">
-        <v>7025.543332458004</v>
+        <v>1069.170787577493</v>
       </c>
       <c r="F27" t="n">
-        <v>12605.13226837616</v>
+        <v>3195.021406916168</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.1097108296855151</v>
+        <v>-0.09451259919386637</v>
       </c>
       <c r="H27" t="n">
-        <v>21925.73538015443</v>
+        <v>3460.468125600244</v>
       </c>
       <c r="I27" t="n">
-        <v>9830.934588235679</v>
+        <v>1157.67631650427</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>[-2.04924257e+08 -4.04818357e+07 -3.92261461e+07 -8.80302196e+08
- -1.23875492e+09]</t>
+          <t>[-19499066.67106559 -14767069.44021334  -8504116.66669209
+  -6537410.25886478 -10566535.20464054]</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>[-0.09520012 -0.00099768 -0.04041298 -0.14193917 -0.2700042 ]</t>
+          <t>[-0.0916692  -0.08289308 -0.10395192 -0.10213464 -0.09191416]</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>[ -7667.43979455  -4786.52320417  -4234.73977455 -13381.79287811
- -19084.17728978]</t>
+          <t>[-1464.40370569 -1227.6787365  -1050.18505607  -929.53914799
+ -1116.57493627]</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>target_enc</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Regressao Linear</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.2151351320811613</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1353.714277909558</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2713.827896903203</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.2261286210895828</v>
+      </c>
+      <c r="H28" t="n">
+        <v>2869.428867047494</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1424.285494767785</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>[-12121383.25559279 -10597178.50815331  -6575017.18656238
+  -5103573.08375127  -6770958.08116759]</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>[0.32137569 0.22289176 0.14647186 0.13959436 0.30030944]</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>[-1616.55615288 -1531.19960295 -1378.9845694  -1273.6386828
+ -1321.04846581]</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>target_enc</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Ridge</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.2151351244256742</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1353.714274915116</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2713.827910138395</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.2262926134424211</v>
+      </c>
+      <c r="H29" t="n">
+        <v>2869.152327664155</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1423.963967582059</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>[-12121383.36307953 -10597178.67703185  -6575017.1366707
+  -5103573.08073685  -6763023.13918426]</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>[0.32137568 0.22289175 0.14647187 0.13959436 0.30112941]</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>[-1616.55614477 -1531.19961808 -1378.98456003 -1273.6386799
+ -1319.44083513]</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>target_enc</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Lasso</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.2151337252722975</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1353.704964324053</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2713.830329064193</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.2262922940011489</v>
+      </c>
+      <c r="H30" t="n">
+        <v>2869.154657511771</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1423.961919386605</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>[-12121448.40508131 -10597211.5067596   -6574996.96024227
+  -5103562.17754795  -6763023.19397631]</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>[0.32137204 0.22288934 0.14647449 0.1395962  0.3011294 ]</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>[-1616.55473921 -1531.20037551 -1378.98033214 -1273.63593694
+ -1319.43821314]</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>target_enc</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ElasticNet</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.2151283959786779</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1353.703851732317</v>
+      </c>
+      <c r="F31" t="n">
+        <v>2713.839542591753</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.2262908957679086</v>
+      </c>
+      <c r="H31" t="n">
+        <v>2869.158770465312</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1423.961635234111</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>[-12121488.40702494 -10597308.71738622  -6574973.30080047
+  -5103565.76488847  -6763024.06059001]</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>[0.3213698  0.22288221 0.14647756 0.13959559 0.30112931]</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>[-1616.54997464 -1531.21015355 -1378.97610368 -1273.63536687
+ -1319.43657743]</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>target_enc</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Arvore de Decisao</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.4041314771086232</v>
+      </c>
+      <c r="E32" t="n">
+        <v>997.799838619823</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2364.613037400586</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.3271962187563799</v>
+      </c>
+      <c r="H32" t="n">
+        <v>2698.224600950643</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1032.993860803483</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>[-12631462.8871277   -8105823.20984309  -6128714.34295046
+  -4312558.60123907  -5223520.94471598]</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>[0.29281851 0.40558687 0.20440814 0.2729506  0.46021696]</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>[-1298.02948104 -1046.28633633 -1008.33504472  -856.70410835
+  -955.61433357]</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>target_enc</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.6093548127577726</v>
+      </c>
+      <c r="E33" t="n">
+        <v>830.9452233459065</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1914.591368902418</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.4616535934528895</v>
+      </c>
+      <c r="H33" t="n">
+        <v>2401.358985134706</v>
+      </c>
+      <c r="I33" t="n">
+        <v>972.3248904826581</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>[-8465459.54801179 -7859881.64784857 -5936938.45760444 -2938657.25034407
+ -3631687.97362708]</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>[0.52605519 0.42362217 0.2293033  0.50457508 0.62471222]</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>[-1234.44051268  -997.1900636   -990.94309748  -789.19059461
+  -849.86018404]</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>target_enc</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Gradient Boosting</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.5364465606965185</v>
+      </c>
+      <c r="E34" t="n">
+        <v>955.409578864356</v>
+      </c>
+      <c r="F34" t="n">
+        <v>2085.617976592639</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.4547953726601358</v>
+      </c>
+      <c r="H34" t="n">
+        <v>2409.939575127463</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1004.404426024213</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>[-7460443.15022223 -8383881.39672952 -5980321.47643747 -2631321.02257785
+ -4583076.73286061]</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>[0.58232175 0.38519642 0.22367159 0.55638855 0.52639855]</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>[-1207.51618497 -1098.22839731  -985.07727316  -784.03454296
+  -947.16573172]</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>target_enc</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.6722469110140918</v>
+      </c>
+      <c r="E35" t="n">
+        <v>786.9423864195361</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1753.711922128728</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.4951040695046956</v>
+      </c>
+      <c r="H35" t="n">
+        <v>2299.455416267803</v>
+      </c>
+      <c r="I35" t="n">
+        <v>891.1694868626251</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>[-7020741.80841314 -6435855.07660991 -6166614.86102991 -2372180.03225054
+ -4442084.27871317]</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>[0.60693875 0.52804834 0.19948813 0.60007684 0.54096829]</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>[-1043.50841331  -889.88865766  -999.17830294  -708.64908749
+  -814.62297292]</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>target_enc</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>LightGBM</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.5886526019691458</v>
+      </c>
+      <c r="E36" t="n">
+        <v>888.9458033539776</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1964.668286851007</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.4345551015969569</v>
+      </c>
+      <c r="H36" t="n">
+        <v>2457.995271877928</v>
+      </c>
+      <c r="I36" t="n">
+        <v>988.7524469525212</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>[-8305785.31017234 -8468924.72357711 -5968428.89544332 -2987278.20156378
+ -4478286.6521147 ]</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>[0.53499467 0.37896005 0.22521541 0.49637813 0.53722725]</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>[-1174.92135479 -1063.7984548  -1015.29585149  -767.79254253
+  -921.95403116]</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>target_enc</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>CatBoost</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.6807925560122159</v>
+      </c>
+      <c r="E37" t="n">
+        <v>770.6039449606109</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1730.698283691551</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.4932270687087408</v>
+      </c>
+      <c r="H37" t="n">
+        <v>2294.832233137671</v>
+      </c>
+      <c r="I37" t="n">
+        <v>886.1324749463098</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>[-6160670.56549688 -7300930.3583402  -6239559.85972736 -2428264.25987763
+ -4201849.84779608]</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>[0.65509045 0.46461097 0.19001886 0.59062166 0.5657934 ]</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>[-1001.74417197  -942.94473103  -915.58441216  -728.30094257
+  -842.08811699]</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>target_enc</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>SVR (Linear Kernel)</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.08819746262530814</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1032.315985447924</v>
+      </c>
+      <c r="F38" t="n">
+        <v>2925.063212400676</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.09941979342267349</v>
+      </c>
+      <c r="H38" t="n">
+        <v>3149.973063863226</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1098.054323226097</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>[-16169160.4231522  -12595660.48153706  -6873545.06299052
+  -5176252.59882984  -8797032.9488098 ]</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>[0.09475799 0.07633985 0.10771882 0.1273414  0.09094092]</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>[-1402.18867659 -1165.96039401 -1010.09484744  -861.71160986
+ -1050.31608823]</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>target_enc</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>SVR (RBF Kernel)</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>-0.02463559736730758</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1018.507498266477</v>
+      </c>
+      <c r="F39" t="n">
+        <v>3100.770171424251</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-0.03846166879091495</v>
+      </c>
+      <c r="H39" t="n">
+        <v>3377.17814777256</v>
+      </c>
+      <c r="I39" t="n">
+        <v>1106.576692047303</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>[-18707260.58306427 -14180484.26265982  -8025001.68475249
+  -6102066.1949062  -10011848.48357972]</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>[-0.04733937 -0.03987784 -0.04175617 -0.02874047 -0.03459449]</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>[-1408.7561976  -1180.56893913 -1008.0167926   -866.06244442
+ -1069.47908649]</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Dataset 1</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>target_enc</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>SVR (Sigmoid Kernel)</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>-0.1914093078160795</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1302.146527895432</v>
+      </c>
+      <c r="F40" t="n">
+        <v>3343.607971889892</v>
+      </c>
+      <c r="G40" t="n">
+        <v>-0.1712356254359423</v>
+      </c>
+      <c r="H40" t="n">
+        <v>3569.421289693199</v>
+      </c>
+      <c r="I40" t="n">
+        <v>1328.948740621766</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>[-20479564.56162303 -15580388.85061814  -9248744.24224749
+  -7134905.37752636 -11260238.68456027]</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>[-0.14656307 -0.14253511 -0.20061488 -0.20286567 -0.1635994 ]</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>[-1620.87236774 -1405.04251677 -1236.15275298 -1108.82957604
+ -1273.84648957]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new encoder (OneHot with PCA)
</commit_message>
<xml_diff>
--- a/Jupyter/Python/resultados_regressao.xlsx
+++ b/Jupyter/Python/resultados_regressao.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G261"/>
+  <dimension ref="A1:G326"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.322398366557731</v>
+        <v>0.3203696550767509</v>
       </c>
       <c r="E8" t="n">
-        <v>1180.441402094499</v>
+        <v>1181.942584118529</v>
       </c>
       <c r="F8" t="n">
-        <v>2537.589887347104</v>
+        <v>2541.38576828115</v>
       </c>
       <c r="G8" t="n">
-        <v>2.220590041630822</v>
+        <v>2.219760455317013</v>
       </c>
     </row>
     <row r="9">
@@ -998,16 +998,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.257420349152697</v>
+        <v>0.2573778295203104</v>
       </c>
       <c r="E21" t="n">
-        <v>1361.505547025442</v>
+        <v>1360.075832579008</v>
       </c>
       <c r="F21" t="n">
-        <v>3545.10932844516</v>
+        <v>3545.210822330384</v>
       </c>
       <c r="G21" t="n">
-        <v>2.262269180471062</v>
+        <v>2.262185706310029</v>
       </c>
     </row>
     <row r="22">
@@ -1349,16 +1349,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>-0.05012804455984687</v>
+        <v>-0.05421823327147846</v>
       </c>
       <c r="E34" t="n">
-        <v>1259.273692538387</v>
+        <v>1258.278033431012</v>
       </c>
       <c r="F34" t="n">
-        <v>3143.073443878885</v>
+        <v>3149.188540885376</v>
       </c>
       <c r="G34" t="n">
-        <v>2.39647220656875</v>
+        <v>2.3966713918949</v>
       </c>
     </row>
     <row r="35">
@@ -1700,16 +1700,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.09707942583007978</v>
+        <v>0.0993202871358837</v>
       </c>
       <c r="E47" t="n">
-        <v>1040.516282801572</v>
+        <v>1037.162742812388</v>
       </c>
       <c r="F47" t="n">
-        <v>2382.197829061965</v>
+        <v>2379.239932616053</v>
       </c>
       <c r="G47" t="n">
-        <v>2.260960130694174</v>
+        <v>2.260734302578673</v>
       </c>
     </row>
     <row r="48">
@@ -2065,16 +2065,16 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.1566925242451652</v>
+        <v>0.1557123846153666</v>
       </c>
       <c r="E60" t="n">
-        <v>1210.434231114975</v>
+        <v>1209.364798235234</v>
       </c>
       <c r="F60" t="n">
-        <v>2901.992622183278</v>
+        <v>2903.756266028241</v>
       </c>
       <c r="G60" t="n">
-        <v>2.285072889841202</v>
+        <v>2.284837964025154</v>
       </c>
     </row>
     <row r="61">
@@ -2428,16 +2428,16 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0.2191436555894121</v>
+        <v>0.2131585368715174</v>
       </c>
       <c r="E73" t="n">
-        <v>1273.525936432737</v>
+        <v>1287.453859489324</v>
       </c>
       <c r="F73" t="n">
-        <v>2724.079540625129</v>
+        <v>2734.499393814607</v>
       </c>
       <c r="G73" t="n">
-        <v>2.535473438659026</v>
+        <v>2.549313863433032</v>
       </c>
     </row>
     <row r="74">
@@ -2779,16 +2779,16 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0.2443605540569769</v>
+        <v>0.2446963164717784</v>
       </c>
       <c r="E86" t="n">
-        <v>1403.396986637805</v>
+        <v>1401.762166380502</v>
       </c>
       <c r="F86" t="n">
-        <v>3576.147486268379</v>
+        <v>3575.352881555679</v>
       </c>
       <c r="G86" t="n">
-        <v>2.465965092291587</v>
+        <v>2.464964051417502</v>
       </c>
     </row>
     <row r="87">
@@ -3130,16 +3130,16 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>0.3463894401027767</v>
+        <v>0.3533782728015001</v>
       </c>
       <c r="E99" t="n">
-        <v>1152.827889415388</v>
+        <v>1146.32787344184</v>
       </c>
       <c r="F99" t="n">
-        <v>2479.66453651548</v>
+        <v>2466.371807766017</v>
       </c>
       <c r="G99" t="n">
-        <v>2.54822809350866</v>
+        <v>2.54638560107847</v>
       </c>
     </row>
     <row r="100">
@@ -3481,16 +3481,16 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>0.1697402477217747</v>
+        <v>0.1696168718745271</v>
       </c>
       <c r="E112" t="n">
-        <v>1065.998695318327</v>
+        <v>1065.6075747525</v>
       </c>
       <c r="F112" t="n">
-        <v>2284.336308666318</v>
+        <v>2284.506027514843</v>
       </c>
       <c r="G112" t="n">
-        <v>2.537834088092289</v>
+        <v>2.537925866443591</v>
       </c>
     </row>
     <row r="113">
@@ -3846,16 +3846,16 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>0.2449084743677351</v>
+        <v>0.2452124995048308</v>
       </c>
       <c r="E125" t="n">
-        <v>1223.937376951064</v>
+        <v>1225.287868516042</v>
       </c>
       <c r="F125" t="n">
-        <v>2766.056968018826</v>
+        <v>2765.182527662786</v>
       </c>
       <c r="G125" t="n">
-        <v>2.52187517813789</v>
+        <v>2.524647345593149</v>
       </c>
     </row>
     <row r="126">
@@ -4209,16 +4209,16 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>0.3836603125510701</v>
+        <v>0.3843468651814392</v>
       </c>
       <c r="E138" t="n">
-        <v>1048.836545540809</v>
+        <v>1048.16851226923</v>
       </c>
       <c r="F138" t="n">
-        <v>2420.161119960637</v>
+        <v>2418.812812373364</v>
       </c>
       <c r="G138" t="n">
-        <v>2.181798564296466</v>
+        <v>2.181526273238971</v>
       </c>
     </row>
     <row r="139">
@@ -4560,16 +4560,16 @@
         </is>
       </c>
       <c r="D151" t="n">
-        <v>0.3621398940226591</v>
+        <v>0.3650737309589819</v>
       </c>
       <c r="E151" t="n">
-        <v>1257.995412805749</v>
+        <v>1256.591259993101</v>
       </c>
       <c r="F151" t="n">
-        <v>3285.646463546463</v>
+        <v>3278.08159101023</v>
       </c>
       <c r="G151" t="n">
-        <v>2.167965154060535</v>
+        <v>2.168053439215266</v>
       </c>
     </row>
     <row r="152">
@@ -4911,16 +4911,16 @@
         </is>
       </c>
       <c r="D164" t="n">
-        <v>0.4811507298691712</v>
+        <v>0.4943645853005236</v>
       </c>
       <c r="E164" t="n">
-        <v>966.5347090898459</v>
+        <v>961.9960783216304</v>
       </c>
       <c r="F164" t="n">
-        <v>2209.296506937023</v>
+        <v>2180.982309865845</v>
       </c>
       <c r="G164" t="n">
-        <v>2.281778779944087</v>
+        <v>2.281502254908425</v>
       </c>
     </row>
     <row r="165">
@@ -5265,7 +5265,7 @@
         <v>0.3097904393178633</v>
       </c>
       <c r="E177" t="n">
-        <v>882.4528999002562</v>
+        <v>882.4528999002563</v>
       </c>
       <c r="F177" t="n">
         <v>2082.780655540951</v>
@@ -5627,16 +5627,16 @@
         </is>
       </c>
       <c r="D190" t="n">
-        <v>0.384185343940191</v>
+        <v>0.3883939051897021</v>
       </c>
       <c r="E190" t="n">
-        <v>1038.954891834165</v>
+        <v>1037.302187621054</v>
       </c>
       <c r="F190" t="n">
-        <v>2499.471186496269</v>
+        <v>2490.164342197598</v>
       </c>
       <c r="G190" t="n">
-        <v>2.180890879244097</v>
+        <v>2.18077574650949</v>
       </c>
     </row>
     <row r="191">
@@ -5990,16 +5990,16 @@
         </is>
       </c>
       <c r="D203" t="n">
-        <v>0.2854704898193183</v>
+        <v>0.2832307229418557</v>
       </c>
       <c r="E203" t="n">
-        <v>1253.355766698755</v>
+        <v>1253.782903093457</v>
       </c>
       <c r="F203" t="n">
-        <v>2605.819308389157</v>
+        <v>2609.900218361937</v>
       </c>
       <c r="G203" t="n">
-        <v>2.389761925181495</v>
+        <v>2.391713698839453</v>
       </c>
     </row>
     <row r="204">
@@ -6341,16 +6341,16 @@
         </is>
       </c>
       <c r="D216" t="n">
-        <v>0.2896309526528934</v>
+        <v>0.2949525608941385</v>
       </c>
       <c r="E216" t="n">
-        <v>1363.865618191831</v>
+        <v>1362.34020622945</v>
       </c>
       <c r="F216" t="n">
-        <v>3467.369510314597</v>
+        <v>3454.357492302452</v>
       </c>
       <c r="G216" t="n">
-        <v>2.422947803709899</v>
+        <v>2.421854576172256</v>
       </c>
     </row>
     <row r="217">
@@ -6692,16 +6692,16 @@
         </is>
       </c>
       <c r="D229" t="n">
-        <v>0.3612140865665294</v>
+        <v>0.3556752241499839</v>
       </c>
       <c r="E229" t="n">
-        <v>1177.805583961522</v>
+        <v>1179.944786216126</v>
       </c>
       <c r="F229" t="n">
-        <v>2451.382413350284</v>
+        <v>2461.987346389159</v>
       </c>
       <c r="G229" t="n">
-        <v>2.502448199402619</v>
+        <v>2.506090725547989</v>
       </c>
     </row>
     <row r="230">
@@ -7043,16 +7043,16 @@
         </is>
       </c>
       <c r="D242" t="n">
-        <v>0.2900748765861877</v>
+        <v>0.2957908001956221</v>
       </c>
       <c r="E242" t="n">
-        <v>990.5421856076148</v>
+        <v>988.5080915780369</v>
       </c>
       <c r="F242" t="n">
-        <v>2112.318111517046</v>
+        <v>2103.797318349993</v>
       </c>
       <c r="G242" t="n">
-        <v>2.392809798886114</v>
+        <v>2.392633794343006</v>
       </c>
     </row>
     <row r="243">
@@ -7408,16 +7408,16 @@
         </is>
       </c>
       <c r="D255" t="n">
-        <v>0.3065976014062322</v>
+        <v>0.3074123270454</v>
       </c>
       <c r="E255" t="n">
-        <v>1196.392288614931</v>
+        <v>1196.143996779268</v>
       </c>
       <c r="F255" t="n">
-        <v>2659.222335892771</v>
+        <v>2657.510593850885</v>
       </c>
       <c r="G255" t="n">
-        <v>2.426991931795031</v>
+        <v>2.428073198725676</v>
       </c>
     </row>
     <row r="256">
@@ -7592,6 +7592,1787 @@
       </c>
       <c r="G261" t="n">
         <v>2.238367660785931</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B262" t="n">
+        <v>1</v>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>Regressao Linear</t>
+        </is>
+      </c>
+      <c r="D262" t="n">
+        <v>0.2295887809690887</v>
+      </c>
+      <c r="E262" t="n">
+        <v>1499.014782236917</v>
+      </c>
+      <c r="F262" t="n">
+        <v>2705.798876140491</v>
+      </c>
+      <c r="G262" t="n">
+        <v>3.000586959540698</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>1</v>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>Ridge</t>
+        </is>
+      </c>
+      <c r="D263" t="n">
+        <v>0.2314380954479228</v>
+      </c>
+      <c r="E263" t="n">
+        <v>1487.222589265751</v>
+      </c>
+      <c r="F263" t="n">
+        <v>2702.549391073327</v>
+      </c>
+      <c r="G263" t="n">
+        <v>2.990359506166595</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>1</v>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>Lasso</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>0.2340582459313095</v>
+      </c>
+      <c r="E264" t="n">
+        <v>1475.181017945082</v>
+      </c>
+      <c r="F264" t="n">
+        <v>2697.93874650482</v>
+      </c>
+      <c r="G264" t="n">
+        <v>2.948561455193562</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>1</v>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>ElasticNet</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>0.09550655220327797</v>
+      </c>
+      <c r="E265" t="n">
+        <v>1455.732262893529</v>
+      </c>
+      <c r="F265" t="n">
+        <v>2931.817449748508</v>
+      </c>
+      <c r="G265" t="n">
+        <v>2.746125940581579</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>1</v>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>Arvore de Decisao</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>0.1409819043110194</v>
+      </c>
+      <c r="E266" t="n">
+        <v>1172.858051427704</v>
+      </c>
+      <c r="F266" t="n">
+        <v>2857.165313582948</v>
+      </c>
+      <c r="G266" t="n">
+        <v>1.939173247692426</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>1</v>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>0.3320881814402206</v>
+      </c>
+      <c r="E267" t="n">
+        <v>1123.429540230176</v>
+      </c>
+      <c r="F267" t="n">
+        <v>2519.380577382539</v>
+      </c>
+      <c r="G267" t="n">
+        <v>2.008250484825088</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>1</v>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>Gradient Boosting</t>
+        </is>
+      </c>
+      <c r="D268" t="n">
+        <v>0.3256212835557628</v>
+      </c>
+      <c r="E268" t="n">
+        <v>1160.174352106995</v>
+      </c>
+      <c r="F268" t="n">
+        <v>2531.547849314308</v>
+      </c>
+      <c r="G268" t="n">
+        <v>2.296401060659067</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B269" t="n">
+        <v>1</v>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="D269" t="n">
+        <v>0.27343059716458</v>
+      </c>
+      <c r="E269" t="n">
+        <v>1138.182970425431</v>
+      </c>
+      <c r="F269" t="n">
+        <v>2627.68175308389</v>
+      </c>
+      <c r="G269" t="n">
+        <v>2.098841853107741</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>1</v>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>LightGBM</t>
+        </is>
+      </c>
+      <c r="D270" t="n">
+        <v>0.3562633920288275</v>
+      </c>
+      <c r="E270" t="n">
+        <v>1134.512605124896</v>
+      </c>
+      <c r="F270" t="n">
+        <v>2473.365600990243</v>
+      </c>
+      <c r="G270" t="n">
+        <v>2.341437840758826</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>1</v>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>CatBoost</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>0.440186284406497</v>
+      </c>
+      <c r="E271" t="n">
+        <v>993.063003244401</v>
+      </c>
+      <c r="F271" t="n">
+        <v>2306.513389638585</v>
+      </c>
+      <c r="G271" t="n">
+        <v>2.046788105305075</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>1</v>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>SVR (Linear Kernel)</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>-0.02522404221319108</v>
+      </c>
+      <c r="E272" t="n">
+        <v>1083.811696808333</v>
+      </c>
+      <c r="F272" t="n">
+        <v>3121.358154622474</v>
+      </c>
+      <c r="G272" t="n">
+        <v>1.889392273956243</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>1</v>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>SVR (RBF Kernel)</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>-0.08799331017859968</v>
+      </c>
+      <c r="E273" t="n">
+        <v>1141.821766044464</v>
+      </c>
+      <c r="F273" t="n">
+        <v>3215.491199454842</v>
+      </c>
+      <c r="G273" t="n">
+        <v>1.958425942422332</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>1</v>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>SVR (Sigmoid Kernel)</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>-0.08212903363332313</v>
+      </c>
+      <c r="E274" t="n">
+        <v>1139.221821293339</v>
+      </c>
+      <c r="F274" t="n">
+        <v>3206.813752959269</v>
+      </c>
+      <c r="G274" t="n">
+        <v>2.020044363394809</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>2</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>Regressao Linear</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>0.209348005263679</v>
+      </c>
+      <c r="E275" t="n">
+        <v>1559.430785528611</v>
+      </c>
+      <c r="F275" t="n">
+        <v>3658.05976402323</v>
+      </c>
+      <c r="G275" t="n">
+        <v>2.759143516689199</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>2</v>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>Ridge</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>0.2088350938368916</v>
+      </c>
+      <c r="E276" t="n">
+        <v>1553.191758142023</v>
+      </c>
+      <c r="F276" t="n">
+        <v>3659.246099144266</v>
+      </c>
+      <c r="G276" t="n">
+        <v>2.746658785398421</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>2</v>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>Lasso</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>0.2077959974995865</v>
+      </c>
+      <c r="E277" t="n">
+        <v>1547.434149078099</v>
+      </c>
+      <c r="F277" t="n">
+        <v>3661.648292128223</v>
+      </c>
+      <c r="G277" t="n">
+        <v>2.739754188470988</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>2</v>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>ElasticNet</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>0.0695759382416461</v>
+      </c>
+      <c r="E278" t="n">
+        <v>1563.976442758627</v>
+      </c>
+      <c r="F278" t="n">
+        <v>3968.245913208488</v>
+      </c>
+      <c r="G278" t="n">
+        <v>2.629611206538204</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>2</v>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>Arvore de Decisao</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>-0.3140299462960423</v>
+      </c>
+      <c r="E279" t="n">
+        <v>1734.96707690901</v>
+      </c>
+      <c r="F279" t="n">
+        <v>4715.858249082165</v>
+      </c>
+      <c r="G279" t="n">
+        <v>2.151713185292054</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>2</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>0.197836309035945</v>
+      </c>
+      <c r="E280" t="n">
+        <v>1368.076250409658</v>
+      </c>
+      <c r="F280" t="n">
+        <v>3684.593750764102</v>
+      </c>
+      <c r="G280" t="n">
+        <v>2.065558134019752</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>2</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>Gradient Boosting</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>0.1735805033922124</v>
+      </c>
+      <c r="E281" t="n">
+        <v>1396.957992243103</v>
+      </c>
+      <c r="F281" t="n">
+        <v>3739.886207518868</v>
+      </c>
+      <c r="G281" t="n">
+        <v>2.237129958457857</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>2</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>0.1412779789975371</v>
+      </c>
+      <c r="E282" t="n">
+        <v>1406.163634386153</v>
+      </c>
+      <c r="F282" t="n">
+        <v>3812.276667725093</v>
+      </c>
+      <c r="G282" t="n">
+        <v>2.104237204456869</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>2</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>LightGBM</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>0.2642568305156586</v>
+      </c>
+      <c r="E283" t="n">
+        <v>1279.84755953895</v>
+      </c>
+      <c r="F283" t="n">
+        <v>3528.752757266131</v>
+      </c>
+      <c r="G283" t="n">
+        <v>2.235680918904583</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>2</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>CatBoost</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>0.2912897172143961</v>
+      </c>
+      <c r="E284" t="n">
+        <v>1214.266951078179</v>
+      </c>
+      <c r="F284" t="n">
+        <v>3463.318861439393</v>
+      </c>
+      <c r="G284" t="n">
+        <v>2.094436070902707</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>2</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>SVR (Linear Kernel)</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>-0.007499683514692768</v>
+      </c>
+      <c r="E285" t="n">
+        <v>1236.080814126876</v>
+      </c>
+      <c r="F285" t="n">
+        <v>4129.339307233821</v>
+      </c>
+      <c r="G285" t="n">
+        <v>1.820633904165713</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>2</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>SVR (RBF Kernel)</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>-0.06364458142559526</v>
+      </c>
+      <c r="E286" t="n">
+        <v>1290.293647722228</v>
+      </c>
+      <c r="F286" t="n">
+        <v>4242.837288807447</v>
+      </c>
+      <c r="G286" t="n">
+        <v>1.933686567837928</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>2</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>SVR (Sigmoid Kernel)</t>
+        </is>
+      </c>
+      <c r="D287" t="n">
+        <v>-0.05828289658719576</v>
+      </c>
+      <c r="E287" t="n">
+        <v>1291.434412863649</v>
+      </c>
+      <c r="F287" t="n">
+        <v>4232.130001064194</v>
+      </c>
+      <c r="G287" t="n">
+        <v>2.085253988306097</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>3</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>Regressao Linear</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>0.2803648696001587</v>
+      </c>
+      <c r="E288" t="n">
+        <v>1408.83758496359</v>
+      </c>
+      <c r="F288" t="n">
+        <v>2601.893875828968</v>
+      </c>
+      <c r="G288" t="n">
+        <v>2.875355978645969</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>3</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>Ridge</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>0.2826744682686956</v>
+      </c>
+      <c r="E289" t="n">
+        <v>1398.104039373749</v>
+      </c>
+      <c r="F289" t="n">
+        <v>2597.715258276866</v>
+      </c>
+      <c r="G289" t="n">
+        <v>2.863569199116419</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B290" t="n">
+        <v>3</v>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>Lasso</t>
+        </is>
+      </c>
+      <c r="D290" t="n">
+        <v>0.2855885485144231</v>
+      </c>
+      <c r="E290" t="n">
+        <v>1387.359376045542</v>
+      </c>
+      <c r="F290" t="n">
+        <v>2592.433378484723</v>
+      </c>
+      <c r="G290" t="n">
+        <v>2.855025657421919</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>3</v>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>ElasticNet</t>
+        </is>
+      </c>
+      <c r="D291" t="n">
+        <v>0.104553818506691</v>
+      </c>
+      <c r="E291" t="n">
+        <v>1412.670878807696</v>
+      </c>
+      <c r="F291" t="n">
+        <v>2902.372465120357</v>
+      </c>
+      <c r="G291" t="n">
+        <v>2.818128776936377</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>3</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Arvore de Decisao</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>0.03743535622595651</v>
+      </c>
+      <c r="E292" t="n">
+        <v>1186.729125366266</v>
+      </c>
+      <c r="F292" t="n">
+        <v>3009.181294749545</v>
+      </c>
+      <c r="G292" t="n">
+        <v>2.06759338974217</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>3</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="D293" t="n">
+        <v>0.406822766002737</v>
+      </c>
+      <c r="E293" t="n">
+        <v>1070.690523010228</v>
+      </c>
+      <c r="F293" t="n">
+        <v>2362.248805802767</v>
+      </c>
+      <c r="G293" t="n">
+        <v>2.110783667531934</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>3</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Gradient Boosting</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>0.4031188607618331</v>
+      </c>
+      <c r="E294" t="n">
+        <v>1077.666044407498</v>
+      </c>
+      <c r="F294" t="n">
+        <v>2369.612481677912</v>
+      </c>
+      <c r="G294" t="n">
+        <v>2.50162590320169</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>3</v>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>0.4141341813962379</v>
+      </c>
+      <c r="E295" t="n">
+        <v>1000.838159350645</v>
+      </c>
+      <c r="F295" t="n">
+        <v>2347.645300336291</v>
+      </c>
+      <c r="G295" t="n">
+        <v>2.176315322521002</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>3</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>LightGBM</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>0.4628947861482892</v>
+      </c>
+      <c r="E296" t="n">
+        <v>1022.375330709813</v>
+      </c>
+      <c r="F296" t="n">
+        <v>2247.82804275159</v>
+      </c>
+      <c r="G296" t="n">
+        <v>2.310851548473315</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B297" t="n">
+        <v>3</v>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>CatBoost</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>0.5220645701245448</v>
+      </c>
+      <c r="E297" t="n">
+        <v>933.3538653211011</v>
+      </c>
+      <c r="F297" t="n">
+        <v>2120.401066793753</v>
+      </c>
+      <c r="G297" t="n">
+        <v>2.208935901820831</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B298" t="n">
+        <v>3</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>SVR (Linear Kernel)</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>-0.003209371869600242</v>
+      </c>
+      <c r="E298" t="n">
+        <v>976.7580664153428</v>
+      </c>
+      <c r="F298" t="n">
+        <v>3072.056445903278</v>
+      </c>
+      <c r="G298" t="n">
+        <v>1.846148072838379</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B299" t="n">
+        <v>3</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>SVR (RBF Kernel)</t>
+        </is>
+      </c>
+      <c r="D299" t="n">
+        <v>-0.06151146680750674</v>
+      </c>
+      <c r="E299" t="n">
+        <v>1026.42303804225</v>
+      </c>
+      <c r="F299" t="n">
+        <v>3160.063035363304</v>
+      </c>
+      <c r="G299" t="n">
+        <v>1.945100493387643</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B300" t="n">
+        <v>3</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>SVR (Sigmoid Kernel)</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>-0.05485010147588087</v>
+      </c>
+      <c r="E300" t="n">
+        <v>1029.870440955709</v>
+      </c>
+      <c r="F300" t="n">
+        <v>3150.132166202746</v>
+      </c>
+      <c r="G300" t="n">
+        <v>2.066878139423097</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B301" t="n">
+        <v>4</v>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>Regressao Linear</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>0.1754972193220675</v>
+      </c>
+      <c r="E301" t="n">
+        <v>1316.741068301994</v>
+      </c>
+      <c r="F301" t="n">
+        <v>2276.40280627935</v>
+      </c>
+      <c r="G301" t="n">
+        <v>3.055086825456224</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B302" t="n">
+        <v>4</v>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Ridge</t>
+        </is>
+      </c>
+      <c r="D302" t="n">
+        <v>0.1806226126401214</v>
+      </c>
+      <c r="E302" t="n">
+        <v>1304.887752992983</v>
+      </c>
+      <c r="F302" t="n">
+        <v>2269.316324085688</v>
+      </c>
+      <c r="G302" t="n">
+        <v>3.023077365595401</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B303" t="n">
+        <v>4</v>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Lasso</t>
+        </is>
+      </c>
+      <c r="D303" t="n">
+        <v>0.1842154203003483</v>
+      </c>
+      <c r="E303" t="n">
+        <v>1294.822664676999</v>
+      </c>
+      <c r="F303" t="n">
+        <v>2264.335606770375</v>
+      </c>
+      <c r="G303" t="n">
+        <v>3.029621618851422</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B304" t="n">
+        <v>4</v>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>ElasticNet</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>0.1031266005859006</v>
+      </c>
+      <c r="E304" t="n">
+        <v>1209.629947941855</v>
+      </c>
+      <c r="F304" t="n">
+        <v>2374.207221761627</v>
+      </c>
+      <c r="G304" t="n">
+        <v>2.62617812551097</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B305" t="n">
+        <v>4</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Arvore de Decisao</t>
+        </is>
+      </c>
+      <c r="D305" t="n">
+        <v>-0.4816898013391051</v>
+      </c>
+      <c r="E305" t="n">
+        <v>1159.95996298203</v>
+      </c>
+      <c r="F305" t="n">
+        <v>3051.628735708698</v>
+      </c>
+      <c r="G305" t="n">
+        <v>2.102177254835716</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B306" t="n">
+        <v>4</v>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>0.2191506490807835</v>
+      </c>
+      <c r="E306" t="n">
+        <v>891.1673319615646</v>
+      </c>
+      <c r="F306" t="n">
+        <v>2215.321063337053</v>
+      </c>
+      <c r="G306" t="n">
+        <v>1.907222447548962</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B307" t="n">
+        <v>4</v>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Gradient Boosting</t>
+        </is>
+      </c>
+      <c r="D307" t="n">
+        <v>0.233450671907882</v>
+      </c>
+      <c r="E307" t="n">
+        <v>944.739719157889</v>
+      </c>
+      <c r="F307" t="n">
+        <v>2194.942277355609</v>
+      </c>
+      <c r="G307" t="n">
+        <v>2.288717398921437</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B308" t="n">
+        <v>4</v>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>0.1413147999797839</v>
+      </c>
+      <c r="E308" t="n">
+        <v>936.6556004986055</v>
+      </c>
+      <c r="F308" t="n">
+        <v>2323.111415027236</v>
+      </c>
+      <c r="G308" t="n">
+        <v>1.928526623842519</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B309" t="n">
+        <v>4</v>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>LightGBM</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>0.3556582021123225</v>
+      </c>
+      <c r="E309" t="n">
+        <v>850.9808945985552</v>
+      </c>
+      <c r="F309" t="n">
+        <v>2012.385605937034</v>
+      </c>
+      <c r="G309" t="n">
+        <v>2.287237224291951</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B310" t="n">
+        <v>4</v>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>CatBoost</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>0.3842073787494874</v>
+      </c>
+      <c r="E310" t="n">
+        <v>804.8144645256762</v>
+      </c>
+      <c r="F310" t="n">
+        <v>1967.298633627645</v>
+      </c>
+      <c r="G310" t="n">
+        <v>2.059861226533194</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B311" t="n">
+        <v>4</v>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>SVR (Linear Kernel)</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>0.01099531148697019</v>
+      </c>
+      <c r="E311" t="n">
+        <v>845.5807218084664</v>
+      </c>
+      <c r="F311" t="n">
+        <v>2493.171910325541</v>
+      </c>
+      <c r="G311" t="n">
+        <v>1.821550119849438</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B312" t="n">
+        <v>4</v>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>SVR (RBF Kernel)</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>-0.07733643796432799</v>
+      </c>
+      <c r="E312" t="n">
+        <v>902.6199681504281</v>
+      </c>
+      <c r="F312" t="n">
+        <v>2602.128410618114</v>
+      </c>
+      <c r="G312" t="n">
+        <v>1.810325748496983</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B313" t="n">
+        <v>4</v>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>SVR (Sigmoid Kernel)</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>-0.06638527053087384</v>
+      </c>
+      <c r="E313" t="n">
+        <v>901.3829399139114</v>
+      </c>
+      <c r="F313" t="n">
+        <v>2588.869260583583</v>
+      </c>
+      <c r="G313" t="n">
+        <v>1.923544738883135</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>Regressao Linear</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>0.2236997187887485</v>
+      </c>
+      <c r="E314" t="n">
+        <v>1446.006055257778</v>
+      </c>
+      <c r="F314" t="n">
+        <v>2810.53883056801</v>
+      </c>
+      <c r="G314" t="n">
+        <v>2.922543320083023</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>Ridge</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>0.2258925675484078</v>
+      </c>
+      <c r="E315" t="n">
+        <v>1435.851534943627</v>
+      </c>
+      <c r="F315" t="n">
+        <v>2807.206768145037</v>
+      </c>
+      <c r="G315" t="n">
+        <v>2.905916214069209</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Lasso</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>0.2279145530614169</v>
+      </c>
+      <c r="E316" t="n">
+        <v>1426.19930193643</v>
+      </c>
+      <c r="F316" t="n">
+        <v>2804.089005972035</v>
+      </c>
+      <c r="G316" t="n">
+        <v>2.893240729984472</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>ElasticNet</t>
+        </is>
+      </c>
+      <c r="D317" t="n">
+        <v>0.09319072738437892</v>
+      </c>
+      <c r="E317" t="n">
+        <v>1410.502383100427</v>
+      </c>
+      <c r="F317" t="n">
+        <v>3044.160762459745</v>
+      </c>
+      <c r="G317" t="n">
+        <v>2.705011012391782</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Arvore de Decisao</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>-0.1543256217745429</v>
+      </c>
+      <c r="E318" t="n">
+        <v>1313.628554171253</v>
+      </c>
+      <c r="F318" t="n">
+        <v>3408.458398280839</v>
+      </c>
+      <c r="G318" t="n">
+        <v>2.065164269390591</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>0.2889744763899215</v>
+      </c>
+      <c r="E319" t="n">
+        <v>1113.340911402907</v>
+      </c>
+      <c r="F319" t="n">
+        <v>2695.386049321615</v>
+      </c>
+      <c r="G319" t="n">
+        <v>2.022953683481434</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>Gradient Boosting</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>0.2839428299044226</v>
+      </c>
+      <c r="E320" t="n">
+        <v>1144.884526978871</v>
+      </c>
+      <c r="F320" t="n">
+        <v>2708.997203966674</v>
+      </c>
+      <c r="G320" t="n">
+        <v>2.330968580310012</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>XGBoost</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>0.2425393893845347</v>
+      </c>
+      <c r="E321" t="n">
+        <v>1120.460091165209</v>
+      </c>
+      <c r="F321" t="n">
+        <v>2777.678784043128</v>
+      </c>
+      <c r="G321" t="n">
+        <v>2.076980250982033</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>LightGBM</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>0.3597683027012745</v>
+      </c>
+      <c r="E322" t="n">
+        <v>1071.929097493054</v>
+      </c>
+      <c r="F322" t="n">
+        <v>2565.58300173625</v>
+      </c>
+      <c r="G322" t="n">
+        <v>2.293801883107169</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>CatBoost</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>0.4094369876237313</v>
+      </c>
+      <c r="E323" t="n">
+        <v>986.3745710423392</v>
+      </c>
+      <c r="F323" t="n">
+        <v>2464.382987874844</v>
+      </c>
+      <c r="G323" t="n">
+        <v>2.102505326140452</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>SVR (Linear Kernel)</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>-0.006234446527628473</v>
+      </c>
+      <c r="E324" t="n">
+        <v>1035.557824789754</v>
+      </c>
+      <c r="F324" t="n">
+        <v>3203.981454521278</v>
+      </c>
+      <c r="G324" t="n">
+        <v>1.844431092702443</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>SVR (RBF Kernel)</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>-0.07262144909400742</v>
+      </c>
+      <c r="E325" t="n">
+        <v>1090.289604989842</v>
+      </c>
+      <c r="F325" t="n">
+        <v>3305.129983560927</v>
+      </c>
+      <c r="G325" t="n">
+        <v>1.911884688036221</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>onehot_pca</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Média</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>SVR (Sigmoid Kernel)</t>
+        </is>
+      </c>
+      <c r="D326" t="n">
+        <v>-0.0654118255568184</v>
+      </c>
+      <c r="E326" t="n">
+        <v>1090.477403756652</v>
+      </c>
+      <c r="F326" t="n">
+        <v>3294.486295202448</v>
+      </c>
+      <c r="G326" t="n">
+        <v>2.023930307501784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>